<commit_message>
adjusted version number; rebuilt model
</commit_message>
<xml_diff>
--- a/dist/COSAS.xlsx
+++ b/dist/COSAS.xlsx
@@ -31,7 +31,7 @@
     <t>Reference Tables</t>
   </si>
   <si>
-    <t>The Unified Molgenis Data Model (UMDM) (v1.1.3, 2022-03-02)</t>
+    <t>The Unified Molgenis Data Model (UMDM) (v1.2.0, 2022-06-07)</t>
   </si>
   <si>
     <t>Lookup tables for the Unified Molgenis Data Model (UMDM) (v1.2.0, 2022-06-07)</t>
@@ -1801,517 +1801,517 @@
     <t>https://www.w3.org/TR/vocab-dcat-3/#Class:Catalog</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C20826</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25398</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0000071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GO_0001894</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25412</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/FIX_0000704</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0001921</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C63536</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171003</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/topic_3168</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/PATO_0020000</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C117655</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C61512</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DUO_0000001</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0500027</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16735</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C103264</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25294</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001902</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C15607</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70713</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/SNOMEDCT/723506003</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171105</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_2340</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16977</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/MESH/D005783</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C172217</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171103</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171193</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C176763</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C20826</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0500027</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25398</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/DUO_0000001</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C15607</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GO_0001894</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0001921</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0000071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0001902</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/GSSO_009418</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C103264</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_2340</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70713</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/GENEPIO_0000085</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171003</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C61512</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C117655</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16977</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171103</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171193</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25412</t>
-  </si>
-  <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171105</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16735</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C172217</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25294</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/FIX_0000704</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/MESH/D005783</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/topic_3168</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/SNOMEDCT/723506003</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C63536</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C73427</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83017</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_001083</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001891</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C166209</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0000689</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_3273</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142704</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93495</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/HL7/C0442737</t>
+  </si>
+  <si>
+    <t>https://w3id.org/fair-genomes/resource/FG_0000003</t>
+  </si>
+  <si>
+    <t>https://w3id.org/reproduceme#wasUpdatedBy</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25737</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C69208</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25688</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C135383</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000036</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C50996</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45330</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000118</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93400</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/SNOMEDCT/423493009</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C67073</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171252</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171004</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25164</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000006</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45262</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C21480</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C48297</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C153145</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70810</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164021</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000178</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C154307</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/valid</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C89336</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25173</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16493</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C153362</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176373</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171192</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C87853</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C69199</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/RO_0000056</t>
+  </si>
+  <si>
+    <t>http://www.orpha.net/ORDO/Orphanet_C023</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171337</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C47922</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000035</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0001094</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_001330</t>
+  </si>
+  <si>
+    <t>http://purl.allotrope.org/ontologies/role#AFRL_0000010</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000044</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C156426</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93629</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C90353</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164339</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C117142</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C94324</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C17730</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164567</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83322</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C53190</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000090</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000037</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176375</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C17003</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1000589</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C71384</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0000089</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C155320</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164024</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C68615</t>
+  </si>
+  <si>
+    <t>https://w3id.org/fair-genomes/resource/FG_0000001</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_3914</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C19924</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142702</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/HL7/C0332241</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93529</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176342</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DUO_0000017</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C69216</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0000069</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164566</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171276</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C132299</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000100</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C115505</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0010199</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C43361</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83142</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25393</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25714</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171192</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C21480</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C135383</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164021</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93400</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93529</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C153362</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93495</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C153145</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93629</t>
-  </si>
-  <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0000689</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C155320</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C43361</t>
-  </si>
-  <si>
-    <t>http://purl.org/dc/terms/valid</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C87853</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C73427</t>
-  </si>
-  <si>
     <t>https://w3id.org/fair-genomes/resource/FG_0000002</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C19924</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0000089</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171276</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C69216</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000006</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171252</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C17730</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25461</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16493</t>
-  </si>
-  <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0010199</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_001330</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C48297</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/HL7/C0332241</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164567</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C156426</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ICO_0000036</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
-  </si>
-  <si>
-    <t>https://w3id.org/fair-genomes/resource/FG_0000001</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_001083</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176373</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142702</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000035</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0001094</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_3273</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/RO_0000056</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C90353</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C132299</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25688</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C154307</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70810</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C94324</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_000090</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25164</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C53190</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C69199</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C115505</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83322</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25737</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ICO_0000178</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83142</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/SNOMEDCT/423493009</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C67073</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ICO_0000044</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0000069</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0000118</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25173</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25393</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000100</t>
-  </si>
-  <si>
-    <t>http://purl.allotrope.org/ontologies/role#AFRL_0000010</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C68615</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/MS_1000589</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164566</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/HL7/C0442737</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C117142</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171337</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176375</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C47922</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C166209</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000037</t>
-  </si>
-  <si>
-    <t>https://w3id.org/fair-genomes/resource/FG_0000003</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C69208</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142704</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/DUO_0000017</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_3914</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C89336</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0001891</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45330</t>
-  </si>
-  <si>
-    <t>https://w3id.org/reproduceme#wasUpdatedBy</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83017</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164024</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171004</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45262</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C71384</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164339</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176342</t>
-  </si>
-  <si>
-    <t>http://www.orpha.net/ORDO/Orphanet_C023</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C50996</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C17003</t>
-  </si>
-  <si>
     <t>dcat</t>
   </si>
   <si>
+    <t>NCIT</t>
+  </si>
+  <si>
+    <t>GENEPIO</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>FIX</t>
+  </si>
+  <si>
+    <t>EDAM</t>
+  </si>
+  <si>
     <t>PATO</t>
   </si>
   <si>
-    <t>NCIT</t>
+    <t>DUO</t>
   </si>
   <si>
     <t>OBI</t>
   </si>
   <si>
-    <t>DUO</t>
-  </si>
-  <si>
-    <t>GO</t>
-  </si>
-  <si>
-    <t>GENEPIO</t>
+    <t>ExO</t>
+  </si>
+  <si>
+    <t>SNOMEDCT</t>
+  </si>
+  <si>
+    <t>EFO</t>
+  </si>
+  <si>
+    <t>MESH</t>
+  </si>
+  <si>
+    <t>SCDO</t>
   </si>
   <si>
     <t>GSSO</t>
   </si>
   <si>
-    <t>SCDO</t>
-  </si>
-  <si>
-    <t>EDAM</t>
-  </si>
-  <si>
-    <t>EFO</t>
-  </si>
-  <si>
-    <t>ExO</t>
-  </si>
-  <si>
-    <t>FIX</t>
-  </si>
-  <si>
-    <t>MESH</t>
-  </si>
-  <si>
-    <t>SNOMEDCT</t>
+    <t>SIO</t>
+  </si>
+  <si>
+    <t>HL7</t>
+  </si>
+  <si>
+    <t>FG</t>
+  </si>
+  <si>
+    <t>reproduceme</t>
+  </si>
+  <si>
+    <t>ICO</t>
+  </si>
+  <si>
+    <t>OMIABIS</t>
   </si>
   <si>
     <t>DCMI</t>
   </si>
   <si>
-    <t>FG</t>
-  </si>
-  <si>
-    <t>OMIABIS</t>
-  </si>
-  <si>
-    <t>SIO</t>
-  </si>
-  <si>
-    <t>HL7</t>
-  </si>
-  <si>
-    <t>ICO</t>
-  </si>
-  <si>
     <t>RO</t>
   </si>
   <si>
+    <t>Orphanet</t>
+  </si>
+  <si>
     <t>AFO</t>
   </si>
   <si>
     <t>MS</t>
-  </si>
-  <si>
-    <t>reproduceme</t>
-  </si>
-  <si>
-    <t>Orphanet</t>
   </si>
   <si>
     <t>isAssociatedWith</t>
@@ -11331,10 +11331,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>594</v>
@@ -11351,16 +11351,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>595</v>
       </c>
       <c r="D5" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E5" t="s">
         <v>765</v>
@@ -11371,10 +11371,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>596</v>
@@ -11391,10 +11391,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>597</v>
@@ -11411,16 +11411,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>598</v>
       </c>
       <c r="D8" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E8" t="s">
         <v>765</v>
@@ -11431,10 +11431,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>599</v>
@@ -11451,16 +11451,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>600</v>
       </c>
       <c r="D10" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E10" t="s">
         <v>765</v>
@@ -11471,16 +11471,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>601</v>
       </c>
       <c r="D11" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="E11" t="s">
         <v>765</v>
@@ -11491,16 +11491,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>602</v>
       </c>
       <c r="D12" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="E12" t="s">
         <v>765</v>
@@ -11511,16 +11511,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>603</v>
       </c>
       <c r="D13" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="E13" t="s">
         <v>765</v>
@@ -11531,16 +11531,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>604</v>
       </c>
       <c r="D14" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="E14" t="s">
         <v>765</v>
@@ -11551,16 +11551,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>605</v>
       </c>
       <c r="D15" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="E15" t="s">
         <v>765</v>
@@ -11571,16 +11571,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>606</v>
       </c>
       <c r="D16" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="E16" t="s">
         <v>765</v>
@@ -11591,16 +11591,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>607</v>
       </c>
       <c r="D17" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E17" t="s">
         <v>765</v>
@@ -11611,16 +11611,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>608</v>
       </c>
       <c r="D18" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E18" t="s">
         <v>765</v>
@@ -11631,16 +11631,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>609</v>
       </c>
       <c r="D19" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E19" t="s">
         <v>765</v>
@@ -11651,16 +11651,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>610</v>
       </c>
       <c r="D20" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E20" t="s">
         <v>765</v>
@@ -11671,16 +11671,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>611</v>
       </c>
       <c r="D21" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="E21" t="s">
         <v>765</v>
@@ -11691,16 +11691,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>612</v>
       </c>
       <c r="D22" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E22" t="s">
         <v>765</v>
@@ -11711,16 +11711,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>613</v>
       </c>
       <c r="D23" t="s">
-        <v>741</v>
+        <v>747</v>
       </c>
       <c r="E23" t="s">
         <v>765</v>
@@ -11731,16 +11731,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>614</v>
       </c>
       <c r="D24" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E24" t="s">
         <v>765</v>
@@ -11751,16 +11751,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>615</v>
       </c>
       <c r="D25" t="s">
-        <v>741</v>
+        <v>748</v>
       </c>
       <c r="E25" t="s">
         <v>765</v>
@@ -11771,16 +11771,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>616</v>
       </c>
       <c r="D26" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E26" t="s">
         <v>765</v>
@@ -11791,16 +11791,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B27" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>617</v>
       </c>
       <c r="D27" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E27" t="s">
         <v>765</v>
@@ -11811,16 +11811,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>618</v>
       </c>
       <c r="D28" t="s">
-        <v>741</v>
+        <v>749</v>
       </c>
       <c r="E28" t="s">
         <v>765</v>
@@ -11831,16 +11831,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>619</v>
       </c>
       <c r="D29" t="s">
-        <v>749</v>
+        <v>740</v>
       </c>
       <c r="E29" t="s">
         <v>765</v>
@@ -11851,16 +11851,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>620</v>
       </c>
       <c r="D30" t="s">
-        <v>741</v>
+        <v>750</v>
       </c>
       <c r="E30" t="s">
         <v>765</v>
@@ -11871,16 +11871,16 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>621</v>
       </c>
       <c r="D31" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="E31" t="s">
         <v>765</v>
@@ -11891,16 +11891,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>622</v>
       </c>
       <c r="D32" t="s">
-        <v>750</v>
+        <v>740</v>
       </c>
       <c r="E32" t="s">
         <v>765</v>
@@ -11911,16 +11911,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>623</v>
       </c>
       <c r="D33" t="s">
-        <v>741</v>
+        <v>751</v>
       </c>
       <c r="E33" t="s">
         <v>765</v>
@@ -11940,7 +11940,7 @@
         <v>624</v>
       </c>
       <c r="D34" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E34" t="s">
         <v>765</v>
@@ -11951,16 +11951,16 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>625</v>
       </c>
       <c r="D35" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E35" t="s">
         <v>765</v>
@@ -11971,16 +11971,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>626</v>
       </c>
       <c r="D36" t="s">
-        <v>751</v>
+        <v>740</v>
       </c>
       <c r="E36" t="s">
         <v>765</v>
@@ -11991,10 +11991,10 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>627</v>
@@ -12011,16 +12011,16 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>628</v>
       </c>
       <c r="D38" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="E38" t="s">
         <v>765</v>
@@ -12031,10 +12031,10 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>629</v>
@@ -12051,10 +12051,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>630</v>
@@ -12071,16 +12071,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>525</v>
+        <v>433</v>
       </c>
       <c r="B41" t="s">
-        <v>525</v>
+        <v>433</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>631</v>
       </c>
       <c r="D41" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E41" t="s">
         <v>765</v>
@@ -12091,16 +12091,16 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>502</v>
+        <v>127</v>
       </c>
       <c r="B42" t="s">
-        <v>502</v>
+        <v>127</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>632</v>
+        <v>597</v>
       </c>
       <c r="D42" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="E42" t="s">
         <v>765</v>
@@ -12111,13 +12111,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>422</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>422</v>
+        <v>130</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>633</v>
+        <v>601</v>
       </c>
       <c r="D43" t="s">
         <v>741</v>
@@ -12131,16 +12131,16 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>127</v>
+        <v>514</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>514</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>601</v>
+        <v>632</v>
       </c>
       <c r="D44" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="E44" t="s">
         <v>765</v>
@@ -12151,16 +12151,16 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>427</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>427</v>
+        <v>129</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>634</v>
+        <v>603</v>
       </c>
       <c r="D45" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E45" t="s">
         <v>765</v>
@@ -12171,16 +12171,16 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>432</v>
+        <v>521</v>
       </c>
       <c r="B46" t="s">
-        <v>432</v>
+        <v>521</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D46" t="s">
-        <v>741</v>
+        <v>754</v>
       </c>
       <c r="E46" t="s">
         <v>765</v>
@@ -12191,16 +12191,16 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>480</v>
+        <v>492</v>
       </c>
       <c r="B47" t="s">
-        <v>480</v>
+        <v>492</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D47" t="s">
-        <v>741</v>
+        <v>747</v>
       </c>
       <c r="E47" t="s">
         <v>765</v>
@@ -12211,16 +12211,16 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>477</v>
+        <v>507</v>
       </c>
       <c r="B48" t="s">
-        <v>477</v>
+        <v>507</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D48" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E48" t="s">
         <v>765</v>
@@ -12231,16 +12231,16 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="B49" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D49" t="s">
-        <v>741</v>
+        <v>750</v>
       </c>
       <c r="E49" t="s">
         <v>765</v>
@@ -12251,16 +12251,16 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>444</v>
+        <v>471</v>
       </c>
       <c r="B50" t="s">
-        <v>444</v>
+        <v>471</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D50" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="E50" t="s">
         <v>765</v>
@@ -12271,16 +12271,16 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>518</v>
+        <v>449</v>
       </c>
       <c r="B51" t="s">
-        <v>518</v>
+        <v>449</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D51" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E51" t="s">
         <v>765</v>
@@ -12291,16 +12291,16 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>452</v>
+        <v>116</v>
       </c>
       <c r="B52" t="s">
-        <v>452</v>
+        <v>116</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>641</v>
+        <v>608</v>
       </c>
       <c r="D52" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
       <c r="E52" t="s">
         <v>765</v>
@@ -12311,16 +12311,16 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="B53" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D53" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E53" t="s">
         <v>765</v>
@@ -12331,16 +12331,16 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>475</v>
+        <v>513</v>
       </c>
       <c r="B54" t="s">
-        <v>475</v>
+        <v>513</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="D54" t="s">
-        <v>749</v>
+        <v>740</v>
       </c>
       <c r="E54" t="s">
         <v>765</v>
@@ -12351,16 +12351,16 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>493</v>
+        <v>467</v>
       </c>
       <c r="B55" t="s">
-        <v>493</v>
+        <v>467</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D55" t="s">
-        <v>741</v>
+        <v>755</v>
       </c>
       <c r="E55" t="s">
         <v>765</v>
@@ -12371,16 +12371,16 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>487</v>
+        <v>496</v>
       </c>
       <c r="B56" t="s">
-        <v>487</v>
+        <v>496</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="D56" t="s">
-        <v>741</v>
+        <v>756</v>
       </c>
       <c r="E56" t="s">
         <v>765</v>
@@ -12391,16 +12391,16 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
       <c r="B57" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="D57" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="E57" t="s">
         <v>765</v>
@@ -12411,16 +12411,16 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>461</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>461</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>618</v>
+        <v>644</v>
       </c>
       <c r="D58" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E58" t="s">
         <v>765</v>
@@ -12431,16 +12431,16 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="B59" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D59" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E59" t="s">
         <v>765</v>
@@ -12451,16 +12451,16 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>131</v>
+        <v>469</v>
       </c>
       <c r="B60" t="s">
-        <v>131</v>
+        <v>469</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>626</v>
+        <v>646</v>
       </c>
       <c r="D60" t="s">
-        <v>751</v>
+        <v>740</v>
       </c>
       <c r="E60" t="s">
         <v>765</v>
@@ -12471,16 +12471,16 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>433</v>
+        <v>110</v>
       </c>
       <c r="B61" t="s">
-        <v>433</v>
+        <v>110</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>648</v>
+        <v>620</v>
       </c>
       <c r="D61" t="s">
-        <v>741</v>
+        <v>750</v>
       </c>
       <c r="E61" t="s">
         <v>765</v>
@@ -12491,16 +12491,16 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>115</v>
+        <v>427</v>
       </c>
       <c r="B62" t="s">
-        <v>115</v>
+        <v>427</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>621</v>
+        <v>647</v>
       </c>
       <c r="D62" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E62" t="s">
         <v>765</v>
@@ -12511,16 +12511,16 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>494</v>
+        <v>128</v>
       </c>
       <c r="B63" t="s">
-        <v>494</v>
+        <v>128</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>649</v>
+        <v>622</v>
       </c>
       <c r="D63" t="s">
-        <v>755</v>
+        <v>740</v>
       </c>
       <c r="E63" t="s">
         <v>765</v>
@@ -12531,16 +12531,16 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>446</v>
+        <v>121</v>
       </c>
       <c r="B64" t="s">
-        <v>446</v>
+        <v>121</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>650</v>
+        <v>623</v>
       </c>
       <c r="D64" t="s">
-        <v>741</v>
+        <v>751</v>
       </c>
       <c r="E64" t="s">
         <v>765</v>
@@ -12551,16 +12551,16 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>495</v>
+        <v>455</v>
       </c>
       <c r="B65" t="s">
-        <v>495</v>
+        <v>455</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="D65" t="s">
-        <v>745</v>
+        <v>758</v>
       </c>
       <c r="E65" t="s">
         <v>765</v>
@@ -12571,16 +12571,16 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>107</v>
+        <v>476</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>476</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>625</v>
+        <v>649</v>
       </c>
       <c r="D66" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E66" t="s">
         <v>765</v>
@@ -12591,16 +12591,16 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="B67" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D67" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E67" t="s">
         <v>765</v>
@@ -12611,16 +12611,16 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>124</v>
+        <v>522</v>
       </c>
       <c r="B68" t="s">
-        <v>124</v>
+        <v>522</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>597</v>
+        <v>651</v>
       </c>
       <c r="D68" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E68" t="s">
         <v>765</v>
@@ -12631,16 +12631,16 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>490</v>
+        <v>440</v>
       </c>
       <c r="B69" t="s">
-        <v>490</v>
+        <v>440</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D69" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E69" t="s">
         <v>765</v>
@@ -12651,16 +12651,16 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>443</v>
+        <v>518</v>
       </c>
       <c r="B70" t="s">
-        <v>443</v>
+        <v>518</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D70" t="s">
-        <v>756</v>
+        <v>740</v>
       </c>
       <c r="E70" t="s">
         <v>765</v>
@@ -12671,16 +12671,16 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>418</v>
+        <v>516</v>
       </c>
       <c r="B71" t="s">
-        <v>418</v>
+        <v>516</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D71" t="s">
-        <v>741</v>
+        <v>747</v>
       </c>
       <c r="E71" t="s">
         <v>765</v>
@@ -12691,13 +12691,13 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>501</v>
+        <v>132</v>
       </c>
       <c r="B72" t="s">
-        <v>501</v>
+        <v>132</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>656</v>
+        <v>596</v>
       </c>
       <c r="D72" t="s">
         <v>741</v>
@@ -12711,16 +12711,16 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>434</v>
+        <v>480</v>
       </c>
       <c r="B73" t="s">
-        <v>434</v>
+        <v>480</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D73" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E73" t="s">
         <v>765</v>
@@ -12731,16 +12731,16 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>429</v>
+        <v>465</v>
       </c>
       <c r="B74" t="s">
-        <v>429</v>
+        <v>465</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="D74" t="s">
-        <v>741</v>
+        <v>749</v>
       </c>
       <c r="E74" t="s">
         <v>765</v>
@@ -12751,16 +12751,16 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>520</v>
+        <v>488</v>
       </c>
       <c r="B75" t="s">
-        <v>520</v>
+        <v>488</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D75" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E75" t="s">
         <v>765</v>
@@ -12771,16 +12771,16 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>523</v>
+        <v>125</v>
       </c>
       <c r="B76" t="s">
-        <v>523</v>
+        <v>125</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>660</v>
+        <v>594</v>
       </c>
       <c r="D76" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E76" t="s">
         <v>765</v>
@@ -12791,16 +12791,16 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>484</v>
+        <v>501</v>
       </c>
       <c r="B77" t="s">
-        <v>484</v>
+        <v>501</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="D77" t="s">
-        <v>749</v>
+        <v>740</v>
       </c>
       <c r="E77" t="s">
         <v>765</v>
@@ -12811,16 +12811,16 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>437</v>
+        <v>506</v>
       </c>
       <c r="B78" t="s">
-        <v>437</v>
+        <v>506</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="D78" t="s">
-        <v>757</v>
+        <v>740</v>
       </c>
       <c r="E78" t="s">
         <v>765</v>
@@ -12831,16 +12831,16 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
       <c r="B79" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="D79" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E79" t="s">
         <v>765</v>
@@ -12851,16 +12851,16 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>106</v>
+        <v>520</v>
       </c>
       <c r="B80" t="s">
-        <v>106</v>
+        <v>520</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>613</v>
+        <v>661</v>
       </c>
       <c r="D80" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E80" t="s">
         <v>765</v>
@@ -12871,16 +12871,16 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B81" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D81" t="s">
-        <v>758</v>
+        <v>740</v>
       </c>
       <c r="E81" t="s">
         <v>765</v>
@@ -12891,16 +12891,16 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>472</v>
+        <v>131</v>
       </c>
       <c r="B82" t="s">
-        <v>472</v>
+        <v>131</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>665</v>
+        <v>599</v>
       </c>
       <c r="D82" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="E82" t="s">
         <v>765</v>
@@ -12911,16 +12911,16 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>426</v>
+        <v>443</v>
       </c>
       <c r="B83" t="s">
-        <v>426</v>
+        <v>443</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="D83" t="s">
-        <v>741</v>
+        <v>759</v>
       </c>
       <c r="E83" t="s">
         <v>765</v>
@@ -12931,16 +12931,16 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>133</v>
+        <v>454</v>
       </c>
       <c r="B84" t="s">
-        <v>133</v>
+        <v>454</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>616</v>
+        <v>664</v>
       </c>
       <c r="D84" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E84" t="s">
         <v>765</v>
@@ -12951,16 +12951,16 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>455</v>
+        <v>422</v>
       </c>
       <c r="B85" t="s">
-        <v>455</v>
+        <v>422</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D85" t="s">
-        <v>759</v>
+        <v>740</v>
       </c>
       <c r="E85" t="s">
         <v>765</v>
@@ -12971,16 +12971,16 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>519</v>
+        <v>123</v>
       </c>
       <c r="B86" t="s">
-        <v>519</v>
+        <v>123</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>668</v>
+        <v>605</v>
       </c>
       <c r="D86" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="E86" t="s">
         <v>765</v>
@@ -12991,16 +12991,16 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>485</v>
+        <v>106</v>
       </c>
       <c r="B87" t="s">
-        <v>485</v>
+        <v>106</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>669</v>
+        <v>607</v>
       </c>
       <c r="D87" t="s">
-        <v>755</v>
+        <v>740</v>
       </c>
       <c r="E87" t="s">
         <v>765</v>
@@ -13011,16 +13011,16 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="B88" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D88" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E88" t="s">
         <v>765</v>
@@ -13031,16 +13031,16 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>521</v>
+        <v>452</v>
       </c>
       <c r="B89" t="s">
-        <v>521</v>
+        <v>452</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D89" t="s">
-        <v>757</v>
+        <v>740</v>
       </c>
       <c r="E89" t="s">
         <v>765</v>
@@ -13051,16 +13051,16 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>506</v>
+        <v>112</v>
       </c>
       <c r="B90" t="s">
-        <v>506</v>
+        <v>112</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>672</v>
+        <v>611</v>
       </c>
       <c r="D90" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E90" t="s">
         <v>765</v>
@@ -13071,16 +13071,16 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>447</v>
+        <v>425</v>
       </c>
       <c r="B91" t="s">
-        <v>447</v>
+        <v>425</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="D91" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E91" t="s">
         <v>765</v>
@@ -13091,16 +13091,16 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="B92" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="D92" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E92" t="s">
         <v>765</v>
@@ -13111,16 +13111,16 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>509</v>
+        <v>439</v>
       </c>
       <c r="B93" t="s">
-        <v>509</v>
+        <v>439</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="D93" t="s">
-        <v>756</v>
+        <v>740</v>
       </c>
       <c r="E93" t="s">
         <v>765</v>
@@ -13131,16 +13131,16 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>428</v>
+        <v>460</v>
       </c>
       <c r="B94" t="s">
-        <v>428</v>
+        <v>460</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="D94" t="s">
-        <v>745</v>
+        <v>758</v>
       </c>
       <c r="E94" t="s">
         <v>765</v>
@@ -13151,16 +13151,16 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>109</v>
+        <v>483</v>
       </c>
       <c r="B95" t="s">
-        <v>109</v>
+        <v>483</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>624</v>
+        <v>672</v>
       </c>
       <c r="D95" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E95" t="s">
         <v>765</v>
@@ -13171,16 +13171,16 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="B96" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D96" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="E96" t="s">
         <v>765</v>
@@ -13191,16 +13191,16 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B97" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="D97" t="s">
-        <v>760</v>
+        <v>740</v>
       </c>
       <c r="E97" t="s">
         <v>765</v>
@@ -13211,16 +13211,16 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>439</v>
+        <v>115</v>
       </c>
       <c r="B98" t="s">
-        <v>439</v>
+        <v>115</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>679</v>
+        <v>619</v>
       </c>
       <c r="D98" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E98" t="s">
         <v>765</v>
@@ -13231,16 +13231,16 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>431</v>
+        <v>505</v>
       </c>
       <c r="B99" t="s">
-        <v>431</v>
+        <v>505</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="D99" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E99" t="s">
         <v>765</v>
@@ -13251,13 +13251,13 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>123</v>
+        <v>419</v>
       </c>
       <c r="B100" t="s">
-        <v>123</v>
+        <v>419</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>594</v>
+        <v>676</v>
       </c>
       <c r="D100" t="s">
         <v>740</v>
@@ -13271,16 +13271,16 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B101" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>595</v>
+        <v>625</v>
       </c>
       <c r="D101" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E101" t="s">
         <v>765</v>
@@ -13291,16 +13291,16 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>479</v>
+        <v>523</v>
       </c>
       <c r="B102" t="s">
-        <v>479</v>
+        <v>523</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="D102" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E102" t="s">
         <v>765</v>
@@ -13311,16 +13311,16 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>469</v>
+        <v>486</v>
       </c>
       <c r="B103" t="s">
-        <v>469</v>
+        <v>486</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="D103" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E103" t="s">
         <v>765</v>
@@ -13331,16 +13331,16 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>483</v>
+        <v>519</v>
       </c>
       <c r="B104" t="s">
-        <v>483</v>
+        <v>519</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D104" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E104" t="s">
         <v>765</v>
@@ -13351,16 +13351,16 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>425</v>
+        <v>447</v>
       </c>
       <c r="B105" t="s">
-        <v>425</v>
+        <v>447</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="D105" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E105" t="s">
         <v>765</v>
@@ -13371,16 +13371,16 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>463</v>
+        <v>113</v>
       </c>
       <c r="B106" t="s">
-        <v>463</v>
+        <v>113</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>685</v>
+        <v>628</v>
       </c>
       <c r="D106" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E106" t="s">
         <v>765</v>
@@ -13391,16 +13391,16 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>421</v>
+        <v>502</v>
       </c>
       <c r="B107" t="s">
-        <v>421</v>
+        <v>502</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="D107" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E107" t="s">
         <v>765</v>
@@ -13411,16 +13411,16 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="B108" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="D108" t="s">
-        <v>757</v>
+        <v>740</v>
       </c>
       <c r="E108" t="s">
         <v>765</v>
@@ -13431,16 +13431,16 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B109" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>599</v>
+        <v>630</v>
       </c>
       <c r="D109" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="E109" t="s">
         <v>765</v>
@@ -13451,16 +13451,16 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>470</v>
+        <v>504</v>
       </c>
       <c r="B110" t="s">
-        <v>470</v>
+        <v>504</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="D110" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E110" t="s">
         <v>765</v>
@@ -13471,16 +13471,16 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>510</v>
+        <v>436</v>
       </c>
       <c r="B111" t="s">
-        <v>510</v>
+        <v>436</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="D111" t="s">
-        <v>741</v>
+        <v>761</v>
       </c>
       <c r="E111" t="s">
         <v>765</v>
@@ -13491,16 +13491,16 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>504</v>
+        <v>466</v>
       </c>
       <c r="B112" t="s">
-        <v>504</v>
+        <v>466</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="D112" t="s">
-        <v>741</v>
+        <v>762</v>
       </c>
       <c r="E112" t="s">
         <v>765</v>
@@ -13511,16 +13511,16 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>524</v>
+        <v>489</v>
       </c>
       <c r="B113" t="s">
-        <v>524</v>
+        <v>489</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="D113" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E113" t="s">
         <v>765</v>
@@ -13531,16 +13531,16 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>424</v>
+        <v>500</v>
       </c>
       <c r="B114" t="s">
-        <v>424</v>
+        <v>500</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="D114" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E114" t="s">
         <v>765</v>
@@ -13551,16 +13551,16 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B115" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="D115" t="s">
-        <v>741</v>
+        <v>759</v>
       </c>
       <c r="E115" t="s">
         <v>765</v>
@@ -13571,13 +13571,13 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>461</v>
+        <v>428</v>
       </c>
       <c r="B116" t="s">
-        <v>461</v>
+        <v>428</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="D116" t="s">
         <v>741</v>
@@ -13591,16 +13591,16 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>460</v>
+        <v>108</v>
       </c>
       <c r="B117" t="s">
-        <v>460</v>
+        <v>108</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>695</v>
+        <v>598</v>
       </c>
       <c r="D117" t="s">
-        <v>759</v>
+        <v>740</v>
       </c>
       <c r="E117" t="s">
         <v>765</v>
@@ -13611,16 +13611,16 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>112</v>
+        <v>437</v>
       </c>
       <c r="B118" t="s">
-        <v>112</v>
+        <v>437</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>607</v>
+        <v>690</v>
       </c>
       <c r="D118" t="s">
-        <v>741</v>
+        <v>754</v>
       </c>
       <c r="E118" t="s">
         <v>765</v>
@@ -13631,16 +13631,16 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>515</v>
+        <v>481</v>
       </c>
       <c r="B119" t="s">
-        <v>515</v>
+        <v>481</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="D119" t="s">
-        <v>741</v>
+        <v>763</v>
       </c>
       <c r="E119" t="s">
         <v>765</v>
@@ -13651,16 +13651,16 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="B120" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="D120" t="s">
-        <v>753</v>
+        <v>758</v>
       </c>
       <c r="E120" t="s">
         <v>765</v>
@@ -13671,16 +13671,16 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>488</v>
+        <v>426</v>
       </c>
       <c r="B121" t="s">
-        <v>488</v>
+        <v>426</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="D121" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E121" t="s">
         <v>765</v>
@@ -13691,16 +13691,16 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>441</v>
       </c>
       <c r="B122" t="s">
-        <v>120</v>
+        <v>441</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>609</v>
+        <v>694</v>
       </c>
       <c r="D122" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="E122" t="s">
         <v>765</v>
@@ -13711,16 +13711,16 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>114</v>
+        <v>431</v>
       </c>
       <c r="B123" t="s">
-        <v>114</v>
+        <v>431</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>610</v>
+        <v>695</v>
       </c>
       <c r="D123" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E123" t="s">
         <v>765</v>
@@ -13731,16 +13731,16 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>453</v>
+        <v>464</v>
       </c>
       <c r="B124" t="s">
-        <v>453</v>
+        <v>464</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="D124" t="s">
-        <v>759</v>
+        <v>740</v>
       </c>
       <c r="E124" t="s">
         <v>765</v>
@@ -13751,16 +13751,16 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D125" t="s">
-        <v>741</v>
+        <v>747</v>
       </c>
       <c r="E125" t="s">
         <v>765</v>
@@ -13771,16 +13771,16 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>491</v>
+        <v>463</v>
       </c>
       <c r="B126" t="s">
-        <v>491</v>
+        <v>463</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="D126" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="E126" t="s">
         <v>765</v>
@@ -13791,16 +13791,16 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>119</v>
+        <v>512</v>
       </c>
       <c r="B127" t="s">
-        <v>119</v>
+        <v>512</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>617</v>
+        <v>698</v>
       </c>
       <c r="D127" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E127" t="s">
         <v>765</v>
@@ -13811,16 +13811,16 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>516</v>
+        <v>421</v>
       </c>
       <c r="B128" t="s">
-        <v>516</v>
+        <v>421</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D128" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E128" t="s">
         <v>765</v>
@@ -13831,16 +13831,16 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>419</v>
+        <v>434</v>
       </c>
       <c r="B129" t="s">
-        <v>419</v>
+        <v>434</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="D129" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E129" t="s">
         <v>765</v>
@@ -13851,16 +13851,16 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>438</v>
+        <v>472</v>
       </c>
       <c r="B130" t="s">
-        <v>438</v>
+        <v>472</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D130" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E130" t="s">
         <v>765</v>
@@ -13871,16 +13871,16 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>508</v>
+        <v>114</v>
       </c>
       <c r="B131" t="s">
-        <v>508</v>
+        <v>114</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>704</v>
+        <v>617</v>
       </c>
       <c r="D131" t="s">
-        <v>756</v>
+        <v>740</v>
       </c>
       <c r="E131" t="s">
         <v>765</v>
@@ -13891,16 +13891,16 @@
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="s">
-        <v>481</v>
+        <v>511</v>
       </c>
       <c r="B132" t="s">
-        <v>481</v>
+        <v>511</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="D132" t="s">
-        <v>761</v>
+        <v>740</v>
       </c>
       <c r="E132" t="s">
         <v>765</v>
@@ -13911,16 +13911,16 @@
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>423</v>
+        <v>120</v>
       </c>
       <c r="B133" t="s">
-        <v>423</v>
+        <v>120</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>706</v>
+        <v>621</v>
       </c>
       <c r="D133" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="E133" t="s">
         <v>765</v>
@@ -13931,16 +13931,16 @@
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>430</v>
+        <v>510</v>
       </c>
       <c r="B134" t="s">
-        <v>430</v>
+        <v>510</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="D134" t="s">
-        <v>762</v>
+        <v>740</v>
       </c>
       <c r="E134" t="s">
         <v>765</v>
@@ -13951,16 +13951,16 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="B135" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="D135" t="s">
-        <v>741</v>
+        <v>754</v>
       </c>
       <c r="E135" t="s">
         <v>765</v>
@@ -13971,16 +13971,16 @@
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>467</v>
+        <v>445</v>
       </c>
       <c r="B136" t="s">
-        <v>467</v>
+        <v>445</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D136" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="E136" t="s">
         <v>765</v>
@@ -13991,16 +13991,16 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" t="s">
-        <v>512</v>
+        <v>448</v>
       </c>
       <c r="B137" t="s">
-        <v>512</v>
+        <v>448</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="D137" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E137" t="s">
         <v>765</v>
@@ -14011,16 +14011,16 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>517</v>
+        <v>482</v>
       </c>
       <c r="B138" t="s">
-        <v>517</v>
+        <v>482</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="D138" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E138" t="s">
         <v>765</v>
@@ -14031,16 +14031,16 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>489</v>
+        <v>430</v>
       </c>
       <c r="B139" t="s">
-        <v>489</v>
+        <v>430</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="D139" t="s">
-        <v>741</v>
+        <v>764</v>
       </c>
       <c r="E139" t="s">
         <v>765</v>
@@ -14051,16 +14051,16 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="B140" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="D140" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E140" t="s">
         <v>765</v>
@@ -14071,16 +14071,16 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>505</v>
+        <v>119</v>
       </c>
       <c r="B141" t="s">
-        <v>505</v>
+        <v>119</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>714</v>
+        <v>626</v>
       </c>
       <c r="D141" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E141" t="s">
         <v>765</v>
@@ -14091,13 +14091,13 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>125</v>
+        <v>495</v>
       </c>
       <c r="B142" t="s">
-        <v>125</v>
+        <v>495</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>596</v>
+        <v>710</v>
       </c>
       <c r="D142" t="s">
         <v>741</v>
@@ -14111,16 +14111,16 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="B143" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="D143" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E143" t="s">
         <v>765</v>
@@ -14131,16 +14131,16 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>507</v>
+        <v>474</v>
       </c>
       <c r="B144" t="s">
-        <v>507</v>
+        <v>474</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="D144" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E144" t="s">
         <v>765</v>
@@ -14151,16 +14151,16 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>498</v>
+        <v>423</v>
       </c>
       <c r="B145" t="s">
-        <v>498</v>
+        <v>423</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="D145" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E145" t="s">
         <v>765</v>
@@ -14171,13 +14171,13 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>445</v>
+        <v>485</v>
       </c>
       <c r="B146" t="s">
-        <v>445</v>
+        <v>485</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D146" t="s">
         <v>756</v>
@@ -14191,16 +14191,16 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>118</v>
+        <v>418</v>
       </c>
       <c r="B147" t="s">
-        <v>118</v>
+        <v>418</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>600</v>
+        <v>715</v>
       </c>
       <c r="D147" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E147" t="s">
         <v>765</v>
@@ -14211,16 +14211,16 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>130</v>
+        <v>497</v>
       </c>
       <c r="B148" t="s">
-        <v>130</v>
+        <v>497</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>602</v>
+        <v>716</v>
       </c>
       <c r="D148" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E148" t="s">
         <v>765</v>
@@ -14231,16 +14231,16 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
-        <v>132</v>
+        <v>446</v>
       </c>
       <c r="B149" t="s">
-        <v>132</v>
+        <v>446</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>603</v>
+        <v>717</v>
       </c>
       <c r="D149" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="E149" t="s">
         <v>765</v>
@@ -14251,16 +14251,16 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
-        <v>496</v>
+        <v>451</v>
       </c>
       <c r="B150" t="s">
-        <v>496</v>
+        <v>451</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D150" t="s">
-        <v>755</v>
+        <v>740</v>
       </c>
       <c r="E150" t="s">
         <v>765</v>
@@ -14271,16 +14271,16 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
-        <v>122</v>
+        <v>468</v>
       </c>
       <c r="B151" t="s">
-        <v>122</v>
+        <v>468</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>606</v>
+        <v>719</v>
       </c>
       <c r="D151" t="s">
-        <v>746</v>
+        <v>755</v>
       </c>
       <c r="E151" t="s">
         <v>765</v>
@@ -14291,16 +14291,16 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
-        <v>450</v>
+        <v>477</v>
       </c>
       <c r="B152" t="s">
-        <v>450</v>
+        <v>477</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>720</v>
       </c>
       <c r="D152" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E152" t="s">
         <v>765</v>
@@ -14311,16 +14311,16 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>126</v>
+        <v>457</v>
       </c>
       <c r="B153" t="s">
-        <v>126</v>
+        <v>457</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>611</v>
+        <v>721</v>
       </c>
       <c r="D153" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="E153" t="s">
         <v>765</v>
@@ -14331,16 +14331,16 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
-        <v>449</v>
+        <v>424</v>
       </c>
       <c r="B154" t="s">
-        <v>449</v>
+        <v>424</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="D154" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E154" t="s">
         <v>765</v>
@@ -14357,10 +14357,10 @@
         <v>458</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D155" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="E155" t="s">
         <v>765</v>
@@ -14377,10 +14377,10 @@
         <v>134</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="D156" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E156" t="s">
         <v>765</v>
@@ -14391,16 +14391,16 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="B157" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="D157" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="E157" t="s">
         <v>765</v>
@@ -14411,13 +14411,13 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>128</v>
+        <v>491</v>
       </c>
       <c r="B158" t="s">
-        <v>128</v>
+        <v>491</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>615</v>
+        <v>725</v>
       </c>
       <c r="D158" t="s">
         <v>741</v>
@@ -14431,16 +14431,16 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>420</v>
+        <v>473</v>
       </c>
       <c r="B159" t="s">
-        <v>420</v>
+        <v>473</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="D159" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E159" t="s">
         <v>765</v>
@@ -14451,16 +14451,16 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
-        <v>110</v>
+        <v>517</v>
       </c>
       <c r="B160" t="s">
-        <v>110</v>
+        <v>517</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>619</v>
+        <v>727</v>
       </c>
       <c r="D160" t="s">
-        <v>749</v>
+        <v>740</v>
       </c>
       <c r="E160" t="s">
         <v>765</v>
@@ -14471,16 +14471,16 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>492</v>
+        <v>503</v>
       </c>
       <c r="B161" t="s">
-        <v>492</v>
+        <v>503</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="D161" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E161" t="s">
         <v>765</v>
@@ -14491,16 +14491,16 @@
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
-        <v>440</v>
+        <v>479</v>
       </c>
       <c r="B162" t="s">
-        <v>440</v>
+        <v>479</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="D162" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E162" t="s">
         <v>765</v>
@@ -14511,16 +14511,16 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
       <c r="B163" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="D163" t="s">
-        <v>741</v>
+        <v>759</v>
       </c>
       <c r="E163" t="s">
         <v>765</v>
@@ -14531,16 +14531,16 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
-        <v>442</v>
+        <v>107</v>
       </c>
       <c r="B164" t="s">
-        <v>442</v>
+        <v>107</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>728</v>
+        <v>612</v>
       </c>
       <c r="D164" t="s">
-        <v>763</v>
+        <v>740</v>
       </c>
       <c r="E164" t="s">
         <v>765</v>
@@ -14551,16 +14551,16 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>514</v>
+        <v>524</v>
       </c>
       <c r="B165" t="s">
-        <v>514</v>
+        <v>524</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="D165" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E165" t="s">
         <v>765</v>
@@ -14571,16 +14571,16 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
-        <v>474</v>
+        <v>118</v>
       </c>
       <c r="B166" t="s">
-        <v>474</v>
+        <v>118</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>730</v>
+        <v>616</v>
       </c>
       <c r="D166" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E166" t="s">
         <v>765</v>
@@ -14591,16 +14591,16 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="B167" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="D167" t="s">
-        <v>741</v>
+        <v>750</v>
       </c>
       <c r="E167" t="s">
         <v>765</v>
@@ -14611,16 +14611,16 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
-        <v>454</v>
+        <v>487</v>
       </c>
       <c r="B168" t="s">
-        <v>454</v>
+        <v>487</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="D168" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E168" t="s">
         <v>765</v>
@@ -14631,16 +14631,16 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
-        <v>435</v>
+        <v>515</v>
       </c>
       <c r="B169" t="s">
-        <v>435</v>
+        <v>515</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="D169" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E169" t="s">
         <v>765</v>
@@ -14651,16 +14651,16 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" t="s">
-        <v>464</v>
+        <v>109</v>
       </c>
       <c r="B170" t="s">
-        <v>464</v>
+        <v>109</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>734</v>
+        <v>624</v>
       </c>
       <c r="D170" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E170" t="s">
         <v>765</v>
@@ -14671,16 +14671,16 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="B171" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>735</v>
       </c>
       <c r="D171" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E171" t="s">
         <v>765</v>
@@ -14691,16 +14691,16 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" t="s">
-        <v>121</v>
+        <v>525</v>
       </c>
       <c r="B172" t="s">
-        <v>121</v>
+        <v>525</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>627</v>
+        <v>736</v>
       </c>
       <c r="D172" t="s">
-        <v>752</v>
+        <v>740</v>
       </c>
       <c r="E172" t="s">
         <v>765</v>
@@ -14711,16 +14711,16 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" t="s">
-        <v>466</v>
+        <v>494</v>
       </c>
       <c r="B173" t="s">
-        <v>466</v>
+        <v>494</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="D173" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="E173" t="s">
         <v>765</v>
@@ -14731,16 +14731,16 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" t="s">
-        <v>476</v>
+        <v>122</v>
       </c>
       <c r="B174" t="s">
-        <v>476</v>
+        <v>122</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>737</v>
+        <v>629</v>
       </c>
       <c r="D174" t="s">
-        <v>741</v>
+        <v>753</v>
       </c>
       <c r="E174" t="s">
         <v>765</v>
@@ -14751,16 +14751,16 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" t="s">
-        <v>482</v>
+        <v>429</v>
       </c>
       <c r="B175" t="s">
-        <v>482</v>
+        <v>429</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>738</v>
       </c>
       <c r="D175" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E175" t="s">
         <v>765</v>
@@ -14881,7 +14881,7 @@
     <hyperlink ref="F55" r:id="rId108" location="isAssociatedWith"/>
     <hyperlink ref="C56" r:id="rId109"/>
     <hyperlink ref="F56" r:id="rId110" location="isAssociatedWith"/>
-    <hyperlink ref="C57" r:id="rId111"/>
+    <hyperlink ref="C57" r:id="rId111" location="wasUpdatedBy"/>
     <hyperlink ref="F57" r:id="rId112" location="isAssociatedWith"/>
     <hyperlink ref="C58" r:id="rId113"/>
     <hyperlink ref="F58" r:id="rId114" location="isAssociatedWith"/>
@@ -15005,7 +15005,7 @@
     <hyperlink ref="F117" r:id="rId232" location="isAssociatedWith"/>
     <hyperlink ref="C118" r:id="rId233"/>
     <hyperlink ref="F118" r:id="rId234" location="isAssociatedWith"/>
-    <hyperlink ref="C119" r:id="rId235"/>
+    <hyperlink ref="C119" r:id="rId235" location="AFRL_0000010"/>
     <hyperlink ref="F119" r:id="rId236" location="isAssociatedWith"/>
     <hyperlink ref="C120" r:id="rId237"/>
     <hyperlink ref="F120" r:id="rId238" location="isAssociatedWith"/>
@@ -15031,7 +15031,7 @@
     <hyperlink ref="F130" r:id="rId258" location="isAssociatedWith"/>
     <hyperlink ref="C131" r:id="rId259"/>
     <hyperlink ref="F131" r:id="rId260" location="isAssociatedWith"/>
-    <hyperlink ref="C132" r:id="rId261" location="AFRL_0000010"/>
+    <hyperlink ref="C132" r:id="rId261"/>
     <hyperlink ref="F132" r:id="rId262" location="isAssociatedWith"/>
     <hyperlink ref="C133" r:id="rId263"/>
     <hyperlink ref="F133" r:id="rId264" location="isAssociatedWith"/>
@@ -15095,7 +15095,7 @@
     <hyperlink ref="F162" r:id="rId322" location="isAssociatedWith"/>
     <hyperlink ref="C163" r:id="rId323"/>
     <hyperlink ref="F163" r:id="rId324" location="isAssociatedWith"/>
-    <hyperlink ref="C164" r:id="rId325" location="wasUpdatedBy"/>
+    <hyperlink ref="C164" r:id="rId325"/>
     <hyperlink ref="F164" r:id="rId326" location="isAssociatedWith"/>
     <hyperlink ref="C165" r:id="rId327"/>
     <hyperlink ref="F165" r:id="rId328" location="isAssociatedWith"/>

</xml_diff>

<commit_message>
fixed typo in subject ID label
</commit_message>
<xml_diff>
--- a/dist/COSAS.xlsx
+++ b/dist/COSAS.xlsx
@@ -1597,7 +1597,7 @@
     <t>NCIT_C25714</t>
   </si>
   <si>
-    <t>MSN_UMCGnr</t>
+    <t>MDN_UMCGnr</t>
   </si>
   <si>
     <t>Familienr</t>
@@ -1801,16 +1801,103 @@
     <t>https://www.w3.org/TR/vocab-dcat-3/#Class:Catalog</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0000085</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176763</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C103264</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GO_0001894</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25398</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C15607</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_2340</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GSSO_009418</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0001921</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001902</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PATO_0020000</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16977</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/SNOMEDCT/723506003</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70713</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C20826</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25398</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C117655</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16735</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0500027</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171103</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25294</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171003</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/MESH/D005783</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DUO_0000001</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C172217</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/topic_3168</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171105</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C63536</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171193</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/GENEPIO_0000071</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/GO_0001894</t>
+    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25412</t>
@@ -1819,499 +1906,412 @@
     <t>http://purl.obolibrary.org/obo/FIX_0000704</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0001921</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C63536</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171003</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/topic_3168</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/PATO_0020000</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C117655</t>
+    <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C61512</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/DUO_0000001</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0500027</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16735</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C103264</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25294</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0001902</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C15607</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70713</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/SNOMEDCT/723506003</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171105</t>
-  </si>
-  <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_2340</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16977</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/MESH/D005783</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C172217</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171103</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171193</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176763</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GSSO_009418</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0000085</t>
+    <t>https://w3id.org/fair-genomes/resource/FG_0000002</t>
+  </si>
+  <si>
+    <t>https://w3id.org/fair-genomes/resource/FG_0000001</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C154307</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/RO_0000056</t>
+  </si>
+  <si>
+    <t>http://www.orpha.net/ORDO/Orphanet_C023</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83322</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C69199</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83142</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C87853</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25173</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C73427</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142702</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C153362</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C69208</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000118</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000006</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0010199</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93629</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164566</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25164</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45262</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164024</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_3914</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C71384</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164567</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_001330</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000037</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/valid</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25737</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1000589</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25714</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/HL7/C0332241</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C17003</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C47922</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171337</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000100</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45330</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_3273</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C166209</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C153145</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C115505</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/SNOMEDCT/423493009</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C90353</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C68615</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C117142</t>
+  </si>
+  <si>
+    <t>https://w3id.org/fair-genomes/resource/FG_0000003</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000036</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/HL7/C0442737</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C135383</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0000069</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C156426</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0000089</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C155320</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25461</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171252</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000035</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25688</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176375</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C50996</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93400</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C89336</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000178</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171004</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C17730</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_001083</t>
+  </si>
+  <si>
+    <t>https://w3id.org/reproduceme#wasUpdatedBy</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164339</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C132299</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C67073</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171276</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16493</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C83017</t>
   </si>
   <si>
-    <t>http://semanticscience.org/resource/SIO_001083</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C43361</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0000689</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142704</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0001891</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C166209</t>
-  </si>
-  <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0000689</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_3273</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142704</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171192</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C94324</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C53190</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DUO_0000017</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93529</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25393</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176342</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C21480</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C69216</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164021</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C19924</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000044</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70810</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000090</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0001094</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176373</t>
+  </si>
+  <si>
+    <t>http://purl.allotrope.org/ontologies/role#AFRL_0000010</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C48297</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C93495</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/HL7/C0442737</t>
-  </si>
-  <si>
-    <t>https://w3id.org/fair-genomes/resource/FG_0000003</t>
-  </si>
-  <si>
-    <t>https://w3id.org/reproduceme#wasUpdatedBy</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25737</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C69208</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25688</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C135383</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ICO_0000036</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C50996</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45330</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0000118</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93400</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/SNOMEDCT/423493009</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C67073</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171252</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171004</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25164</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000006</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45262</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C21480</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C48297</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C153145</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70810</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164021</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ICO_0000178</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C154307</t>
-  </si>
-  <si>
-    <t>http://purl.org/dc/terms/valid</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C89336</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25173</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16493</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C153362</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176373</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171192</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C87853</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C69199</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/RO_0000056</t>
-  </si>
-  <si>
-    <t>http://www.orpha.net/ORDO/Orphanet_C023</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171337</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C47922</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000035</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0001094</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_001330</t>
-  </si>
-  <si>
-    <t>http://purl.allotrope.org/ontologies/role#AFRL_0000010</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ICO_0000044</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C156426</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93629</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C90353</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164339</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C117142</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C94324</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C17730</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164567</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83322</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C53190</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_000090</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000037</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176375</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C17003</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/MS_1000589</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C71384</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0000089</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C155320</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164024</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C68615</t>
-  </si>
-  <si>
-    <t>https://w3id.org/fair-genomes/resource/FG_0000001</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_3914</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C19924</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142702</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/HL7/C0332241</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93529</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176342</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/DUO_0000017</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C69216</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0000069</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164566</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171276</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C132299</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000100</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C115505</t>
-  </si>
-  <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0010199</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C43361</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83142</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25393</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25714</t>
-  </si>
-  <si>
-    <t>https://w3id.org/fair-genomes/resource/FG_0000002</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25461</t>
-  </si>
-  <si>
     <t>dcat</t>
   </si>
   <si>
+    <t>GENEPIO</t>
+  </si>
+  <si>
     <t>NCIT</t>
   </si>
   <si>
-    <t>GENEPIO</t>
-  </si>
-  <si>
     <t>GO</t>
   </si>
   <si>
+    <t>EDAM</t>
+  </si>
+  <si>
+    <t>GSSO</t>
+  </si>
+  <si>
+    <t>EFO</t>
+  </si>
+  <si>
+    <t>OBI</t>
+  </si>
+  <si>
+    <t>PATO</t>
+  </si>
+  <si>
+    <t>SNOMEDCT</t>
+  </si>
+  <si>
+    <t>MESH</t>
+  </si>
+  <si>
+    <t>DUO</t>
+  </si>
+  <si>
+    <t>ExO</t>
+  </si>
+  <si>
     <t>FIX</t>
   </si>
   <si>
-    <t>EDAM</t>
-  </si>
-  <si>
-    <t>PATO</t>
-  </si>
-  <si>
-    <t>DUO</t>
-  </si>
-  <si>
-    <t>OBI</t>
-  </si>
-  <si>
-    <t>ExO</t>
-  </si>
-  <si>
-    <t>SNOMEDCT</t>
-  </si>
-  <si>
-    <t>EFO</t>
-  </si>
-  <si>
-    <t>MESH</t>
-  </si>
-  <si>
     <t>SCDO</t>
   </si>
   <si>
-    <t>GSSO</t>
+    <t>FG</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>Orphanet</t>
+  </si>
+  <si>
+    <t>OMIABIS</t>
   </si>
   <si>
     <t>SIO</t>
   </si>
   <si>
+    <t>DCMI</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
     <t>HL7</t>
   </si>
   <si>
-    <t>FG</t>
+    <t>ICO</t>
   </si>
   <si>
     <t>reproduceme</t>
   </si>
   <si>
-    <t>ICO</t>
-  </si>
-  <si>
-    <t>OMIABIS</t>
-  </si>
-  <si>
-    <t>DCMI</t>
-  </si>
-  <si>
-    <t>RO</t>
-  </si>
-  <si>
-    <t>Orphanet</t>
-  </si>
-  <si>
     <t>AFO</t>
-  </si>
-  <si>
-    <t>MS</t>
   </si>
   <si>
     <t>isAssociatedWith</t>
@@ -11331,10 +11331,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>594</v>
@@ -11351,16 +11351,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>595</v>
       </c>
       <c r="D5" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E5" t="s">
         <v>765</v>
@@ -11371,10 +11371,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>596</v>
@@ -11411,16 +11411,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>598</v>
       </c>
       <c r="D8" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E8" t="s">
         <v>765</v>
@@ -11431,16 +11431,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>599</v>
       </c>
       <c r="D9" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="E9" t="s">
         <v>765</v>
@@ -11451,16 +11451,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>600</v>
       </c>
       <c r="D10" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="E10" t="s">
         <v>765</v>
@@ -11471,16 +11471,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>601</v>
       </c>
       <c r="D11" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="E11" t="s">
         <v>765</v>
@@ -11491,16 +11491,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>602</v>
       </c>
       <c r="D12" t="s">
-        <v>740</v>
+        <v>745</v>
       </c>
       <c r="E12" t="s">
         <v>765</v>
@@ -11511,10 +11511,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>603</v>
@@ -11531,16 +11531,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>604</v>
       </c>
       <c r="D14" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="E14" t="s">
         <v>765</v>
@@ -11560,7 +11560,7 @@
         <v>605</v>
       </c>
       <c r="D15" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="E15" t="s">
         <v>765</v>
@@ -11571,16 +11571,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>606</v>
       </c>
       <c r="D16" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E16" t="s">
         <v>765</v>
@@ -11591,16 +11591,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>607</v>
       </c>
       <c r="D17" t="s">
-        <v>740</v>
+        <v>748</v>
       </c>
       <c r="E17" t="s">
         <v>765</v>
@@ -11611,16 +11611,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>608</v>
       </c>
       <c r="D18" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="E18" t="s">
         <v>765</v>
@@ -11631,16 +11631,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>609</v>
       </c>
       <c r="D19" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="E19" t="s">
         <v>765</v>
@@ -11651,16 +11651,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>610</v>
       </c>
       <c r="D20" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E20" t="s">
         <v>765</v>
@@ -11671,16 +11671,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>611</v>
       </c>
       <c r="D21" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E21" t="s">
         <v>765</v>
@@ -11691,16 +11691,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>612</v>
       </c>
       <c r="D22" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E22" t="s">
         <v>765</v>
@@ -11711,16 +11711,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>613</v>
       </c>
       <c r="D23" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E23" t="s">
         <v>765</v>
@@ -11731,16 +11731,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>614</v>
       </c>
       <c r="D24" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E24" t="s">
         <v>765</v>
@@ -11751,16 +11751,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>615</v>
       </c>
       <c r="D25" t="s">
-        <v>748</v>
+        <v>741</v>
       </c>
       <c r="E25" t="s">
         <v>765</v>
@@ -11771,16 +11771,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>616</v>
       </c>
       <c r="D26" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E26" t="s">
         <v>765</v>
@@ -11791,16 +11791,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>617</v>
       </c>
       <c r="D27" t="s">
-        <v>740</v>
+        <v>749</v>
       </c>
       <c r="E27" t="s">
         <v>765</v>
@@ -11811,16 +11811,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>618</v>
       </c>
       <c r="D28" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="E28" t="s">
         <v>765</v>
@@ -11831,16 +11831,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>619</v>
       </c>
       <c r="D29" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E29" t="s">
         <v>765</v>
@@ -11851,16 +11851,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>620</v>
       </c>
       <c r="D30" t="s">
-        <v>750</v>
+        <v>741</v>
       </c>
       <c r="E30" t="s">
         <v>765</v>
@@ -11871,16 +11871,16 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>621</v>
       </c>
       <c r="D31" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E31" t="s">
         <v>765</v>
@@ -11891,16 +11891,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>622</v>
       </c>
       <c r="D32" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E32" t="s">
         <v>765</v>
@@ -11911,16 +11911,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>623</v>
       </c>
       <c r="D33" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
       <c r="E33" t="s">
         <v>765</v>
@@ -11931,16 +11931,16 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>624</v>
       </c>
       <c r="D34" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E34" t="s">
         <v>765</v>
@@ -11951,10 +11951,10 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>625</v>
@@ -11971,16 +11971,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>626</v>
       </c>
       <c r="D36" t="s">
-        <v>740</v>
+        <v>751</v>
       </c>
       <c r="E36" t="s">
         <v>765</v>
@@ -11991,16 +11991,16 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>627</v>
       </c>
       <c r="D37" t="s">
-        <v>752</v>
+        <v>741</v>
       </c>
       <c r="E37" t="s">
         <v>765</v>
@@ -12011,16 +12011,16 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B38" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>628</v>
       </c>
       <c r="D38" t="s">
-        <v>740</v>
+        <v>752</v>
       </c>
       <c r="E38" t="s">
         <v>765</v>
@@ -12031,10 +12031,10 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B39" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>629</v>
@@ -12051,10 +12051,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>630</v>
@@ -12071,13 +12071,13 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>433</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
-        <v>433</v>
+        <v>126</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>631</v>
+        <v>594</v>
       </c>
       <c r="D41" t="s">
         <v>740</v>
@@ -12091,16 +12091,16 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>494</v>
       </c>
       <c r="B42" t="s">
-        <v>127</v>
+        <v>494</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>597</v>
+        <v>631</v>
       </c>
       <c r="D42" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="E42" t="s">
         <v>765</v>
@@ -12111,16 +12111,16 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>485</v>
       </c>
       <c r="B43" t="s">
-        <v>130</v>
+        <v>485</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>601</v>
+        <v>632</v>
       </c>
       <c r="D43" t="s">
-        <v>741</v>
+        <v>754</v>
       </c>
       <c r="E43" t="s">
         <v>765</v>
@@ -12131,16 +12131,16 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>514</v>
+        <v>113</v>
       </c>
       <c r="B44" t="s">
-        <v>514</v>
+        <v>113</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>632</v>
+        <v>595</v>
       </c>
       <c r="D44" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E44" t="s">
         <v>765</v>
@@ -12151,16 +12151,16 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>483</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>483</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>603</v>
+        <v>633</v>
       </c>
       <c r="D45" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E45" t="s">
         <v>765</v>
@@ -12171,16 +12171,16 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>521</v>
+        <v>436</v>
       </c>
       <c r="B46" t="s">
-        <v>521</v>
+        <v>436</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D46" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="E46" t="s">
         <v>765</v>
@@ -12191,16 +12191,16 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>492</v>
+        <v>466</v>
       </c>
       <c r="B47" t="s">
-        <v>492</v>
+        <v>466</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="D47" t="s">
-        <v>747</v>
+        <v>756</v>
       </c>
       <c r="E47" t="s">
         <v>765</v>
@@ -12211,16 +12211,16 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="B48" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D48" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E48" t="s">
         <v>765</v>
@@ -12231,16 +12231,16 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>475</v>
+        <v>120</v>
       </c>
       <c r="B49" t="s">
-        <v>475</v>
+        <v>120</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>636</v>
+        <v>600</v>
       </c>
       <c r="D49" t="s">
-        <v>750</v>
+        <v>743</v>
       </c>
       <c r="E49" t="s">
         <v>765</v>
@@ -12251,16 +12251,16 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>471</v>
+        <v>504</v>
       </c>
       <c r="B50" t="s">
-        <v>471</v>
+        <v>504</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>637</v>
       </c>
       <c r="D50" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="E50" t="s">
         <v>765</v>
@@ -12271,16 +12271,16 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>449</v>
+        <v>110</v>
       </c>
       <c r="B51" t="s">
-        <v>449</v>
+        <v>110</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>638</v>
+        <v>602</v>
       </c>
       <c r="D51" t="s">
-        <v>740</v>
+        <v>745</v>
       </c>
       <c r="E51" t="s">
         <v>765</v>
@@ -12291,16 +12291,16 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="D52" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="E52" t="s">
         <v>765</v>
@@ -12311,16 +12311,16 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>444</v>
+        <v>515</v>
       </c>
       <c r="B53" t="s">
-        <v>444</v>
+        <v>515</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D53" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E53" t="s">
         <v>765</v>
@@ -12331,16 +12331,16 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>513</v>
+        <v>462</v>
       </c>
       <c r="B54" t="s">
-        <v>513</v>
+        <v>462</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D54" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E54" t="s">
         <v>765</v>
@@ -12351,16 +12351,16 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>467</v>
+        <v>419</v>
       </c>
       <c r="B55" t="s">
-        <v>467</v>
+        <v>419</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D55" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
       <c r="E55" t="s">
         <v>765</v>
@@ -12371,16 +12371,16 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>496</v>
+        <v>433</v>
       </c>
       <c r="B56" t="s">
-        <v>496</v>
+        <v>433</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D56" t="s">
-        <v>756</v>
+        <v>741</v>
       </c>
       <c r="E56" t="s">
         <v>765</v>
@@ -12391,16 +12391,16 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
       <c r="B57" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D57" t="s">
-        <v>757</v>
+        <v>741</v>
       </c>
       <c r="E57" t="s">
         <v>765</v>
@@ -12411,16 +12411,16 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>461</v>
+        <v>486</v>
       </c>
       <c r="B58" t="s">
-        <v>461</v>
+        <v>486</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D58" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E58" t="s">
         <v>765</v>
@@ -12437,10 +12437,10 @@
         <v>450</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D59" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E59" t="s">
         <v>765</v>
@@ -12451,16 +12451,16 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>469</v>
+        <v>516</v>
       </c>
       <c r="B60" t="s">
-        <v>469</v>
+        <v>516</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D60" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="E60" t="s">
         <v>765</v>
@@ -12471,16 +12471,16 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="B61" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>620</v>
+        <v>610</v>
       </c>
       <c r="D61" t="s">
-        <v>750</v>
+        <v>741</v>
       </c>
       <c r="E61" t="s">
         <v>765</v>
@@ -12491,16 +12491,16 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>427</v>
+        <v>506</v>
       </c>
       <c r="B62" t="s">
-        <v>427</v>
+        <v>506</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D62" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E62" t="s">
         <v>765</v>
@@ -12511,16 +12511,16 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>443</v>
       </c>
       <c r="B63" t="s">
-        <v>128</v>
+        <v>443</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>622</v>
+        <v>647</v>
       </c>
       <c r="D63" t="s">
-        <v>740</v>
+        <v>757</v>
       </c>
       <c r="E63" t="s">
         <v>765</v>
@@ -12531,16 +12531,16 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>121</v>
+        <v>484</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>484</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>623</v>
+        <v>648</v>
       </c>
       <c r="D64" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="E64" t="s">
         <v>765</v>
@@ -12551,16 +12551,16 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>455</v>
+        <v>441</v>
       </c>
       <c r="B65" t="s">
-        <v>455</v>
+        <v>441</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="D65" t="s">
-        <v>758</v>
+        <v>741</v>
       </c>
       <c r="E65" t="s">
         <v>765</v>
@@ -12571,16 +12571,16 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B66" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D66" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E66" t="s">
         <v>765</v>
@@ -12597,10 +12597,10 @@
         <v>498</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="D67" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E67" t="s">
         <v>765</v>
@@ -12611,16 +12611,16 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>522</v>
+        <v>470</v>
       </c>
       <c r="B68" t="s">
-        <v>522</v>
+        <v>470</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="D68" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E68" t="s">
         <v>765</v>
@@ -12631,16 +12631,16 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="B69" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="D69" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E69" t="s">
         <v>765</v>
@@ -12651,16 +12651,16 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>518</v>
+        <v>474</v>
       </c>
       <c r="B70" t="s">
-        <v>518</v>
+        <v>474</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D70" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E70" t="s">
         <v>765</v>
@@ -12671,16 +12671,16 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>516</v>
+        <v>440</v>
       </c>
       <c r="B71" t="s">
-        <v>516</v>
+        <v>440</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="D71" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="E71" t="s">
         <v>765</v>
@@ -12691,16 +12691,16 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>132</v>
+        <v>497</v>
       </c>
       <c r="B72" t="s">
-        <v>132</v>
+        <v>497</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>596</v>
+        <v>656</v>
       </c>
       <c r="D72" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="E72" t="s">
         <v>765</v>
@@ -12711,16 +12711,16 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>480</v>
+        <v>435</v>
       </c>
       <c r="B73" t="s">
-        <v>480</v>
+        <v>435</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="D73" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E73" t="s">
         <v>765</v>
@@ -12731,16 +12731,16 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="B74" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="D74" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="E74" t="s">
         <v>765</v>
@@ -12751,16 +12751,16 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>488</v>
+        <v>437</v>
       </c>
       <c r="B75" t="s">
-        <v>488</v>
+        <v>437</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="D75" t="s">
-        <v>740</v>
+        <v>758</v>
       </c>
       <c r="E75" t="s">
         <v>765</v>
@@ -12771,16 +12771,16 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B76" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>594</v>
+        <v>619</v>
       </c>
       <c r="D76" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E76" t="s">
         <v>765</v>
@@ -12791,16 +12791,16 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>501</v>
+        <v>445</v>
       </c>
       <c r="B77" t="s">
-        <v>501</v>
+        <v>445</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="D77" t="s">
-        <v>740</v>
+        <v>757</v>
       </c>
       <c r="E77" t="s">
         <v>765</v>
@@ -12811,16 +12811,16 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>506</v>
+        <v>456</v>
       </c>
       <c r="B78" t="s">
-        <v>506</v>
+        <v>456</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="D78" t="s">
-        <v>740</v>
+        <v>759</v>
       </c>
       <c r="E78" t="s">
         <v>765</v>
@@ -12831,13 +12831,13 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>478</v>
+        <v>132</v>
       </c>
       <c r="B79" t="s">
-        <v>478</v>
+        <v>132</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>660</v>
+        <v>625</v>
       </c>
       <c r="D79" t="s">
         <v>740</v>
@@ -12851,16 +12851,16 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>520</v>
+        <v>461</v>
       </c>
       <c r="B80" t="s">
-        <v>520</v>
+        <v>461</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="D80" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E80" t="s">
         <v>765</v>
@@ -12871,16 +12871,16 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>470</v>
+        <v>430</v>
       </c>
       <c r="B81" t="s">
-        <v>470</v>
+        <v>430</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D81" t="s">
-        <v>740</v>
+        <v>760</v>
       </c>
       <c r="E81" t="s">
         <v>765</v>
@@ -12897,10 +12897,10 @@
         <v>131</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>599</v>
+        <v>628</v>
       </c>
       <c r="D82" t="s">
-        <v>743</v>
+        <v>752</v>
       </c>
       <c r="E82" t="s">
         <v>765</v>
@@ -12911,16 +12911,16 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>443</v>
+        <v>525</v>
       </c>
       <c r="B83" t="s">
-        <v>443</v>
+        <v>525</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="D83" t="s">
-        <v>759</v>
+        <v>741</v>
       </c>
       <c r="E83" t="s">
         <v>765</v>
@@ -12931,16 +12931,16 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="B84" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="D84" t="s">
-        <v>740</v>
+        <v>761</v>
       </c>
       <c r="E84" t="s">
         <v>765</v>
@@ -12951,16 +12951,16 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>422</v>
+        <v>482</v>
       </c>
       <c r="B85" t="s">
-        <v>422</v>
+        <v>482</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D85" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E85" t="s">
         <v>765</v>
@@ -12971,16 +12971,16 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>123</v>
+        <v>500</v>
       </c>
       <c r="B86" t="s">
-        <v>123</v>
+        <v>500</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>605</v>
+        <v>667</v>
       </c>
       <c r="D86" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="E86" t="s">
         <v>765</v>
@@ -12991,16 +12991,16 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>106</v>
+        <v>519</v>
       </c>
       <c r="B87" t="s">
-        <v>106</v>
+        <v>519</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>607</v>
+        <v>668</v>
       </c>
       <c r="D87" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E87" t="s">
         <v>765</v>
@@ -13011,16 +13011,16 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="B88" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="D88" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E88" t="s">
         <v>765</v>
@@ -13031,16 +13031,16 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>452</v>
+        <v>123</v>
       </c>
       <c r="B89" t="s">
-        <v>452</v>
+        <v>123</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>667</v>
+        <v>605</v>
       </c>
       <c r="D89" t="s">
-        <v>740</v>
+        <v>747</v>
       </c>
       <c r="E89" t="s">
         <v>765</v>
@@ -13051,16 +13051,16 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>112</v>
+        <v>508</v>
       </c>
       <c r="B90" t="s">
-        <v>112</v>
+        <v>508</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>611</v>
+        <v>670</v>
       </c>
       <c r="D90" t="s">
-        <v>740</v>
+        <v>757</v>
       </c>
       <c r="E90" t="s">
         <v>765</v>
@@ -13071,16 +13071,16 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>425</v>
+        <v>522</v>
       </c>
       <c r="B91" t="s">
-        <v>425</v>
+        <v>522</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="D91" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E91" t="s">
         <v>765</v>
@@ -13091,16 +13091,16 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>432</v>
+        <v>471</v>
       </c>
       <c r="B92" t="s">
-        <v>432</v>
+        <v>471</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="D92" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="E92" t="s">
         <v>765</v>
@@ -13111,16 +13111,16 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>439</v>
+        <v>507</v>
       </c>
       <c r="B93" t="s">
-        <v>439</v>
+        <v>507</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="D93" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E93" t="s">
         <v>765</v>
@@ -13131,16 +13131,16 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>460</v>
+        <v>125</v>
       </c>
       <c r="B94" t="s">
-        <v>460</v>
+        <v>125</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>671</v>
+        <v>609</v>
       </c>
       <c r="D94" t="s">
-        <v>758</v>
+        <v>741</v>
       </c>
       <c r="E94" t="s">
         <v>765</v>
@@ -13151,16 +13151,16 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>483</v>
+        <v>452</v>
       </c>
       <c r="B95" t="s">
-        <v>483</v>
+        <v>452</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="D95" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E95" t="s">
         <v>765</v>
@@ -13171,16 +13171,16 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>456</v>
+        <v>524</v>
       </c>
       <c r="B96" t="s">
-        <v>456</v>
+        <v>524</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="D96" t="s">
-        <v>760</v>
+        <v>741</v>
       </c>
       <c r="E96" t="s">
         <v>765</v>
@@ -13191,16 +13191,16 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>420</v>
+        <v>465</v>
       </c>
       <c r="B97" t="s">
-        <v>420</v>
+        <v>465</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="D97" t="s">
-        <v>740</v>
+        <v>748</v>
       </c>
       <c r="E97" t="s">
         <v>765</v>
@@ -13211,16 +13211,16 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>115</v>
+        <v>431</v>
       </c>
       <c r="B98" t="s">
-        <v>115</v>
+        <v>431</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>619</v>
+        <v>677</v>
       </c>
       <c r="D98" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E98" t="s">
         <v>765</v>
@@ -13231,16 +13231,16 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>505</v>
+        <v>423</v>
       </c>
       <c r="B99" t="s">
-        <v>505</v>
+        <v>423</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="D99" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E99" t="s">
         <v>765</v>
@@ -13251,16 +13251,16 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>419</v>
+        <v>512</v>
       </c>
       <c r="B100" t="s">
-        <v>419</v>
+        <v>512</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="D100" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E100" t="s">
         <v>765</v>
@@ -13271,16 +13271,16 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>133</v>
+        <v>496</v>
       </c>
       <c r="B101" t="s">
-        <v>133</v>
+        <v>496</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>625</v>
+        <v>680</v>
       </c>
       <c r="D101" t="s">
-        <v>740</v>
+        <v>754</v>
       </c>
       <c r="E101" t="s">
         <v>765</v>
@@ -13291,16 +13291,16 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>523</v>
+        <v>455</v>
       </c>
       <c r="B102" t="s">
-        <v>523</v>
+        <v>455</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="D102" t="s">
-        <v>740</v>
+        <v>762</v>
       </c>
       <c r="E102" t="s">
         <v>765</v>
@@ -13311,16 +13311,16 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
       <c r="B103" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
       <c r="D103" t="s">
-        <v>740</v>
+        <v>761</v>
       </c>
       <c r="E103" t="s">
         <v>765</v>
@@ -13331,16 +13331,16 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>519</v>
+        <v>116</v>
       </c>
       <c r="B104" t="s">
-        <v>519</v>
+        <v>116</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>679</v>
+        <v>618</v>
       </c>
       <c r="D104" t="s">
-        <v>740</v>
+        <v>750</v>
       </c>
       <c r="E104" t="s">
         <v>765</v>
@@ -13351,16 +13351,16 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
       <c r="B105" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="D105" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E105" t="s">
         <v>765</v>
@@ -13371,13 +13371,13 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>113</v>
+        <v>491</v>
       </c>
       <c r="B106" t="s">
-        <v>113</v>
+        <v>491</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>628</v>
+        <v>684</v>
       </c>
       <c r="D106" t="s">
         <v>740</v>
@@ -13391,16 +13391,16 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>502</v>
+        <v>426</v>
       </c>
       <c r="B107" t="s">
-        <v>502</v>
+        <v>426</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c r="D107" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E107" t="s">
         <v>765</v>
@@ -13411,16 +13411,16 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>462</v>
+        <v>418</v>
       </c>
       <c r="B108" t="s">
-        <v>462</v>
+        <v>418</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="D108" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E108" t="s">
         <v>765</v>
@@ -13431,13 +13431,13 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D109" t="s">
         <v>741</v>
@@ -13451,13 +13451,13 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="B110" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="D110" t="s">
         <v>740</v>
@@ -13471,16 +13471,16 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>436</v>
+        <v>505</v>
       </c>
       <c r="B111" t="s">
-        <v>436</v>
+        <v>505</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="D111" t="s">
-        <v>761</v>
+        <v>741</v>
       </c>
       <c r="E111" t="s">
         <v>765</v>
@@ -13491,16 +13491,16 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>466</v>
+        <v>106</v>
       </c>
       <c r="B112" t="s">
-        <v>466</v>
+        <v>106</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>685</v>
+        <v>630</v>
       </c>
       <c r="D112" t="s">
-        <v>762</v>
+        <v>741</v>
       </c>
       <c r="E112" t="s">
         <v>765</v>
@@ -13511,16 +13511,16 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="B113" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="D113" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E113" t="s">
         <v>765</v>
@@ -13531,16 +13531,16 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>500</v>
+        <v>429</v>
       </c>
       <c r="B114" t="s">
-        <v>500</v>
+        <v>429</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="D114" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E114" t="s">
         <v>765</v>
@@ -13551,16 +13551,16 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>509</v>
+        <v>127</v>
       </c>
       <c r="B115" t="s">
-        <v>509</v>
+        <v>127</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>688</v>
+        <v>597</v>
       </c>
       <c r="D115" t="s">
-        <v>759</v>
+        <v>742</v>
       </c>
       <c r="E115" t="s">
         <v>765</v>
@@ -13571,13 +13571,13 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>428</v>
+        <v>501</v>
       </c>
       <c r="B116" t="s">
-        <v>428</v>
+        <v>501</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D116" t="s">
         <v>741</v>
@@ -13591,16 +13591,16 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D117" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E117" t="s">
         <v>765</v>
@@ -13611,16 +13611,16 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>437</v>
+        <v>128</v>
       </c>
       <c r="B118" t="s">
-        <v>437</v>
+        <v>128</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>690</v>
+        <v>606</v>
       </c>
       <c r="D118" t="s">
-        <v>754</v>
+        <v>741</v>
       </c>
       <c r="E118" t="s">
         <v>765</v>
@@ -13631,16 +13631,16 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>481</v>
+        <v>509</v>
       </c>
       <c r="B119" t="s">
-        <v>481</v>
+        <v>509</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="D119" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="E119" t="s">
         <v>765</v>
@@ -13651,16 +13651,16 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>453</v>
+        <v>469</v>
       </c>
       <c r="B120" t="s">
-        <v>453</v>
+        <v>469</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="D120" t="s">
-        <v>758</v>
+        <v>741</v>
       </c>
       <c r="E120" t="s">
         <v>765</v>
@@ -13671,16 +13671,16 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>426</v>
+        <v>448</v>
       </c>
       <c r="B121" t="s">
-        <v>426</v>
+        <v>448</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="D121" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E121" t="s">
         <v>765</v>
@@ -13691,16 +13691,16 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>441</v>
+        <v>476</v>
       </c>
       <c r="B122" t="s">
-        <v>441</v>
+        <v>476</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="D122" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E122" t="s">
         <v>765</v>
@@ -13711,16 +13711,16 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>431</v>
+        <v>480</v>
       </c>
       <c r="B123" t="s">
-        <v>431</v>
+        <v>480</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="D123" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E123" t="s">
         <v>765</v>
@@ -13731,16 +13731,16 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>464</v>
+        <v>420</v>
       </c>
       <c r="B124" t="s">
-        <v>464</v>
+        <v>420</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="D124" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E124" t="s">
         <v>765</v>
@@ -13751,16 +13751,16 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B125" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D125" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="E125" t="s">
         <v>765</v>
@@ -13771,16 +13771,16 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B126" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="D126" t="s">
-        <v>740</v>
+        <v>762</v>
       </c>
       <c r="E126" t="s">
         <v>765</v>
@@ -13791,16 +13791,16 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>512</v>
+        <v>478</v>
       </c>
       <c r="B127" t="s">
-        <v>512</v>
+        <v>478</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="D127" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E127" t="s">
         <v>765</v>
@@ -13811,16 +13811,16 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="B128" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D128" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E128" t="s">
         <v>765</v>
@@ -13831,16 +13831,16 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>434</v>
+        <v>521</v>
       </c>
       <c r="B129" t="s">
-        <v>434</v>
+        <v>521</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D129" t="s">
-        <v>740</v>
+        <v>758</v>
       </c>
       <c r="E129" t="s">
         <v>765</v>
@@ -13851,16 +13851,16 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>472</v>
+        <v>133</v>
       </c>
       <c r="B130" t="s">
-        <v>472</v>
+        <v>133</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>701</v>
+        <v>614</v>
       </c>
       <c r="D130" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E130" t="s">
         <v>765</v>
@@ -13871,16 +13871,16 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B131" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D131" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E131" t="s">
         <v>765</v>
@@ -13891,16 +13891,16 @@
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="s">
-        <v>511</v>
+        <v>442</v>
       </c>
       <c r="B132" t="s">
-        <v>511</v>
+        <v>442</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>702</v>
       </c>
       <c r="D132" t="s">
-        <v>740</v>
+        <v>763</v>
       </c>
       <c r="E132" t="s">
         <v>765</v>
@@ -13911,16 +13911,16 @@
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>120</v>
+        <v>464</v>
       </c>
       <c r="B133" t="s">
-        <v>120</v>
+        <v>464</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>621</v>
+        <v>703</v>
       </c>
       <c r="D133" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="E133" t="s">
         <v>765</v>
@@ -13931,16 +13931,16 @@
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>510</v>
+        <v>479</v>
       </c>
       <c r="B134" t="s">
-        <v>510</v>
+        <v>479</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="D134" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E134" t="s">
         <v>765</v>
@@ -13951,16 +13951,16 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="s">
-        <v>459</v>
+        <v>121</v>
       </c>
       <c r="B135" t="s">
-        <v>459</v>
+        <v>121</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>704</v>
+        <v>617</v>
       </c>
       <c r="D135" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="E135" t="s">
         <v>765</v>
@@ -13971,16 +13971,16 @@
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>445</v>
+        <v>513</v>
       </c>
       <c r="B136" t="s">
-        <v>445</v>
+        <v>513</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>705</v>
       </c>
       <c r="D136" t="s">
-        <v>759</v>
+        <v>741</v>
       </c>
       <c r="E136" t="s">
         <v>765</v>
@@ -13991,16 +13991,16 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" t="s">
-        <v>448</v>
+        <v>488</v>
       </c>
       <c r="B137" t="s">
-        <v>448</v>
+        <v>488</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>706</v>
       </c>
       <c r="D137" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E137" t="s">
         <v>765</v>
@@ -14011,16 +14011,16 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>482</v>
+        <v>503</v>
       </c>
       <c r="B138" t="s">
-        <v>482</v>
+        <v>503</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>707</v>
       </c>
       <c r="D138" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E138" t="s">
         <v>765</v>
@@ -14031,16 +14031,16 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>430</v>
+        <v>523</v>
       </c>
       <c r="B139" t="s">
-        <v>430</v>
+        <v>523</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>708</v>
       </c>
       <c r="D139" t="s">
-        <v>764</v>
+        <v>741</v>
       </c>
       <c r="E139" t="s">
         <v>765</v>
@@ -14051,16 +14051,16 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>435</v>
+        <v>514</v>
       </c>
       <c r="B140" t="s">
-        <v>435</v>
+        <v>514</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>709</v>
       </c>
       <c r="D140" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E140" t="s">
         <v>765</v>
@@ -14071,16 +14071,16 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>119</v>
+        <v>517</v>
       </c>
       <c r="B141" t="s">
-        <v>119</v>
+        <v>517</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>626</v>
+        <v>710</v>
       </c>
       <c r="D141" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E141" t="s">
         <v>765</v>
@@ -14091,13 +14091,13 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="B142" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="D142" t="s">
         <v>741</v>
@@ -14111,16 +14111,16 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>493</v>
+        <v>424</v>
       </c>
       <c r="B143" t="s">
-        <v>493</v>
+        <v>424</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="D143" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E143" t="s">
         <v>765</v>
@@ -14131,16 +14131,16 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B144" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="D144" t="s">
-        <v>740</v>
+        <v>745</v>
       </c>
       <c r="E144" t="s">
         <v>765</v>
@@ -14151,16 +14151,16 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>423</v>
+        <v>449</v>
       </c>
       <c r="B145" t="s">
-        <v>423</v>
+        <v>449</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D145" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E145" t="s">
         <v>765</v>
@@ -14171,16 +14171,16 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>485</v>
+        <v>112</v>
       </c>
       <c r="B146" t="s">
-        <v>485</v>
+        <v>112</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>714</v>
+        <v>596</v>
       </c>
       <c r="D146" t="s">
-        <v>756</v>
+        <v>741</v>
       </c>
       <c r="E146" t="s">
         <v>765</v>
@@ -14191,16 +14191,16 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>418</v>
+        <v>122</v>
       </c>
       <c r="B147" t="s">
-        <v>418</v>
+        <v>122</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>715</v>
+        <v>601</v>
       </c>
       <c r="D147" t="s">
-        <v>740</v>
+        <v>744</v>
       </c>
       <c r="E147" t="s">
         <v>765</v>
@@ -14211,16 +14211,16 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="B148" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D148" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="E148" t="s">
         <v>765</v>
@@ -14231,16 +14231,16 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
-        <v>446</v>
+        <v>502</v>
       </c>
       <c r="B149" t="s">
-        <v>446</v>
+        <v>502</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D149" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E149" t="s">
         <v>765</v>
@@ -14251,16 +14251,16 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
-        <v>451</v>
+        <v>518</v>
       </c>
       <c r="B150" t="s">
-        <v>451</v>
+        <v>518</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D150" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E150" t="s">
         <v>765</v>
@@ -14271,16 +14271,16 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
-        <v>468</v>
+        <v>421</v>
       </c>
       <c r="B151" t="s">
-        <v>468</v>
+        <v>421</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D151" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
       <c r="E151" t="s">
         <v>765</v>
@@ -14291,16 +14291,16 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
-        <v>477</v>
+        <v>510</v>
       </c>
       <c r="B152" t="s">
-        <v>477</v>
+        <v>510</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D152" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E152" t="s">
         <v>765</v>
@@ -14311,16 +14311,16 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="B153" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D153" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E153" t="s">
         <v>765</v>
@@ -14331,16 +14331,16 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
-        <v>424</v>
+        <v>458</v>
       </c>
       <c r="B154" t="s">
-        <v>424</v>
+        <v>458</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D154" t="s">
-        <v>740</v>
+        <v>750</v>
       </c>
       <c r="E154" t="s">
         <v>765</v>
@@ -14351,13 +14351,13 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
-        <v>458</v>
+        <v>124</v>
       </c>
       <c r="B155" t="s">
-        <v>458</v>
+        <v>124</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>723</v>
+        <v>613</v>
       </c>
       <c r="D155" t="s">
         <v>746</v>
@@ -14371,16 +14371,16 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>134</v>
+        <v>477</v>
       </c>
       <c r="B156" t="s">
-        <v>134</v>
+        <v>477</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>606</v>
+        <v>722</v>
       </c>
       <c r="D156" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E156" t="s">
         <v>765</v>
@@ -14391,16 +14391,16 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>490</v>
+        <v>438</v>
       </c>
       <c r="B157" t="s">
-        <v>490</v>
+        <v>438</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D157" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E157" t="s">
         <v>765</v>
@@ -14411,13 +14411,13 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>491</v>
+        <v>457</v>
       </c>
       <c r="B158" t="s">
-        <v>491</v>
+        <v>457</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D158" t="s">
         <v>741</v>
@@ -14431,16 +14431,16 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>473</v>
+        <v>129</v>
       </c>
       <c r="B159" t="s">
-        <v>473</v>
+        <v>129</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>726</v>
+        <v>616</v>
       </c>
       <c r="D159" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E159" t="s">
         <v>765</v>
@@ -14451,16 +14451,16 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
-        <v>517</v>
+        <v>422</v>
       </c>
       <c r="B160" t="s">
-        <v>517</v>
+        <v>422</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D160" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E160" t="s">
         <v>765</v>
@@ -14471,16 +14471,16 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="B161" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="D161" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E161" t="s">
         <v>765</v>
@@ -14491,16 +14491,16 @@
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
-        <v>479</v>
+        <v>520</v>
       </c>
       <c r="B162" t="s">
-        <v>479</v>
+        <v>520</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="D162" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E162" t="s">
         <v>765</v>
@@ -14511,16 +14511,16 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
-        <v>508</v>
+        <v>439</v>
       </c>
       <c r="B163" t="s">
-        <v>508</v>
+        <v>439</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D163" t="s">
-        <v>759</v>
+        <v>741</v>
       </c>
       <c r="E163" t="s">
         <v>765</v>
@@ -14531,16 +14531,16 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
-        <v>107</v>
+        <v>432</v>
       </c>
       <c r="B164" t="s">
-        <v>107</v>
+        <v>432</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>612</v>
+        <v>729</v>
       </c>
       <c r="D164" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E164" t="s">
         <v>765</v>
@@ -14551,16 +14551,16 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>524</v>
+        <v>446</v>
       </c>
       <c r="B165" t="s">
-        <v>524</v>
+        <v>446</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D165" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E165" t="s">
         <v>765</v>
@@ -14571,16 +14571,16 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B166" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>616</v>
+        <v>622</v>
       </c>
       <c r="D166" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E166" t="s">
         <v>765</v>
@@ -14591,16 +14591,16 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
-        <v>484</v>
+        <v>453</v>
       </c>
       <c r="B167" t="s">
-        <v>484</v>
+        <v>453</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D167" t="s">
-        <v>750</v>
+        <v>762</v>
       </c>
       <c r="E167" t="s">
         <v>765</v>
@@ -14611,16 +14611,16 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
-        <v>487</v>
+        <v>425</v>
       </c>
       <c r="B168" t="s">
-        <v>487</v>
+        <v>425</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D168" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E168" t="s">
         <v>765</v>
@@ -14631,16 +14631,16 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
-        <v>515</v>
+        <v>459</v>
       </c>
       <c r="B169" t="s">
-        <v>515</v>
+        <v>459</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D169" t="s">
-        <v>740</v>
+        <v>758</v>
       </c>
       <c r="E169" t="s">
         <v>765</v>
@@ -14651,13 +14651,13 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" t="s">
-        <v>109</v>
+        <v>428</v>
       </c>
       <c r="B170" t="s">
-        <v>109</v>
+        <v>428</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>624</v>
+        <v>734</v>
       </c>
       <c r="D170" t="s">
         <v>740</v>
@@ -14671,16 +14671,16 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" t="s">
-        <v>438</v>
+        <v>119</v>
       </c>
       <c r="B171" t="s">
-        <v>438</v>
+        <v>119</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>735</v>
+        <v>624</v>
       </c>
       <c r="D171" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E171" t="s">
         <v>765</v>
@@ -14691,16 +14691,16 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" t="s">
-        <v>525</v>
+        <v>447</v>
       </c>
       <c r="B172" t="s">
-        <v>525</v>
+        <v>447</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D172" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E172" t="s">
         <v>765</v>
@@ -14711,16 +14711,16 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="B173" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D173" t="s">
-        <v>756</v>
+        <v>764</v>
       </c>
       <c r="E173" t="s">
         <v>765</v>
@@ -14731,16 +14731,16 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" t="s">
-        <v>122</v>
+        <v>499</v>
       </c>
       <c r="B174" t="s">
-        <v>122</v>
+        <v>499</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>629</v>
+        <v>737</v>
       </c>
       <c r="D174" t="s">
-        <v>753</v>
+        <v>741</v>
       </c>
       <c r="E174" t="s">
         <v>765</v>
@@ -14751,16 +14751,16 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" t="s">
-        <v>429</v>
+        <v>444</v>
       </c>
       <c r="B175" t="s">
-        <v>429</v>
+        <v>444</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>738</v>
       </c>
       <c r="D175" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E175" t="s">
         <v>765</v>
@@ -14881,7 +14881,7 @@
     <hyperlink ref="F55" r:id="rId108" location="isAssociatedWith"/>
     <hyperlink ref="C56" r:id="rId109"/>
     <hyperlink ref="F56" r:id="rId110" location="isAssociatedWith"/>
-    <hyperlink ref="C57" r:id="rId111" location="wasUpdatedBy"/>
+    <hyperlink ref="C57" r:id="rId111"/>
     <hyperlink ref="F57" r:id="rId112" location="isAssociatedWith"/>
     <hyperlink ref="C58" r:id="rId113"/>
     <hyperlink ref="F58" r:id="rId114" location="isAssociatedWith"/>
@@ -15005,7 +15005,7 @@
     <hyperlink ref="F117" r:id="rId232" location="isAssociatedWith"/>
     <hyperlink ref="C118" r:id="rId233"/>
     <hyperlink ref="F118" r:id="rId234" location="isAssociatedWith"/>
-    <hyperlink ref="C119" r:id="rId235" location="AFRL_0000010"/>
+    <hyperlink ref="C119" r:id="rId235"/>
     <hyperlink ref="F119" r:id="rId236" location="isAssociatedWith"/>
     <hyperlink ref="C120" r:id="rId237"/>
     <hyperlink ref="F120" r:id="rId238" location="isAssociatedWith"/>
@@ -15031,7 +15031,7 @@
     <hyperlink ref="F130" r:id="rId258" location="isAssociatedWith"/>
     <hyperlink ref="C131" r:id="rId259"/>
     <hyperlink ref="F131" r:id="rId260" location="isAssociatedWith"/>
-    <hyperlink ref="C132" r:id="rId261"/>
+    <hyperlink ref="C132" r:id="rId261" location="wasUpdatedBy"/>
     <hyperlink ref="F132" r:id="rId262" location="isAssociatedWith"/>
     <hyperlink ref="C133" r:id="rId263"/>
     <hyperlink ref="F133" r:id="rId264" location="isAssociatedWith"/>
@@ -15113,7 +15113,7 @@
     <hyperlink ref="F171" r:id="rId340" location="isAssociatedWith"/>
     <hyperlink ref="C172" r:id="rId341"/>
     <hyperlink ref="F172" r:id="rId342" location="isAssociatedWith"/>
-    <hyperlink ref="C173" r:id="rId343"/>
+    <hyperlink ref="C173" r:id="rId343" location="AFRL_0000010"/>
     <hyperlink ref="F173" r:id="rId344" location="isAssociatedWith"/>
     <hyperlink ref="C174" r:id="rId345"/>
     <hyperlink ref="F174" r:id="rId346" location="isAssociatedWith"/>

</xml_diff>

<commit_message>
changed datatype to text
</commit_message>
<xml_diff>
--- a/dist/COSAS.xlsx
+++ b/dist/COSAS.xlsx
@@ -1804,514 +1804,514 @@
     <t>http://purl.bioontology.org/ontology/MESH/D005783</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25398</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C117655</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_2340</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PATO_0020000</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C15607</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176763</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16735</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DUO_0000001</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C63536</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0000071</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/topic_3168</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C20826</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171003</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70713</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C172217</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25294</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0001921</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171105</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001902</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25412</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GSSO_009418</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0000085</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/SNOMEDCT/723506003</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GO_0001894</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171193</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C103264</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16977</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/FIX_0000704</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C61512</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171103</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/OBI_0500027</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176763</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GO_0001894</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C103264</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C172217</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16977</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171193</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0001921</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171103</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171105</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171003</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/SNOMEDCT/723506003</t>
-  </si>
-  <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GSSO_009418</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C61512</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16735</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0001902</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
   </si>
   <si>
-    <t>http://edamontology.org/topic_3168</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25294</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_2340</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25398</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/DUO_0000001</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/PATO_0020000</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C20826</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/FIX_0000704</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C117655</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0000071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C63536</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C15607</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70713</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25412</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0000085</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C67073</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0000069</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25164</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C69199</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000035</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93400</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C154307</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25714</t>
+  </si>
+  <si>
+    <t>https://w3id.org/reproduceme#wasUpdatedBy</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/valid</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171004</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25688</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142704</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C73427</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C155320</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171337</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C50996</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000118</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25173</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000100</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/RO_0000056</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C19924</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C89336</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45262</t>
+  </si>
+  <si>
+    <t>https://w3id.org/fair-genomes/resource/FG_0000001</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C166209</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
+  </si>
+  <si>
+    <t>http://purl.allotrope.org/ontologies/role#AFRL_0000010</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45330</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000037</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/MS_1000589</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000037</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45330</t>
+    <t>http://semanticscience.org/resource/SIO_001330</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C47922</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C53190</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C71384</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25737</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000044</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C115505</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142702</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C132299</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000036</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164339</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C48297</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/SNOMEDCT/423493009</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DUO_0000017</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70810</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93529</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C43361</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C71384</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176375</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000090</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000178</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C156426</t>
+  </si>
+  <si>
+    <t>https://w3id.org/fair-genomes/resource/FG_0000002</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171192</t>
+  </si>
+  <si>
+    <t>https://w3id.org/fair-genomes/resource/FG_0000003</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0010199</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_001083</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171276</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83322</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171252</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164567</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0000089</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C117142</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83142</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C135383</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0000689</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176373</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164566</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/HL7/C0442737</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0001094</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C17003</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C153362</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C68615</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C94324</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93629</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C90353</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176342</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C153145</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C87853</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C21480</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_3273</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C69216</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_3914</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83017</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164024</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000006</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C69208</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164021</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001891</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16493</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C17730</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93495</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/HL7/C0332241</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25393</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C166209</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C50996</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C117142</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0001891</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C132299</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0001094</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171192</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25737</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C17730</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_3273</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93629</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70810</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C94324</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C19924</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000100</t>
-  </si>
-  <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0010199</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
-  </si>
-  <si>
-    <t>https://w3id.org/fair-genomes/resource/FG_0000003</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ICO_0000178</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93529</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25461</t>
   </si>
   <si>
     <t>http://www.orpha.net/ORDO/Orphanet_C023</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C153362</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C87853</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/DUO_0000017</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C115505</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171337</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C69199</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164566</t>
-  </si>
-  <si>
-    <t>https://w3id.org/fair-genomes/resource/FG_0000001</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C73427</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000035</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C156426</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171252</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C89336</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C17003</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0000118</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_3914</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/RO_0000056</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25714</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/HL7/C0442737</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142704</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25461</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25688</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171004</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164567</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C47922</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142702</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C154307</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C135383</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25164</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16493</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93400</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164021</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83142</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C69216</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176375</t>
-  </si>
-  <si>
-    <t>https://w3id.org/reproduceme#wasUpdatedBy</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C90353</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0000089</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ICO_0000044</t>
-  </si>
-  <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0000689</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C153145</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ICO_0000036</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C155320</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83322</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0000069</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C21480</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C53190</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176373</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/HL7/C0332241</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25173</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_000090</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176342</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000006</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171276</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93495</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164339</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164024</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83017</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/SNOMEDCT/423493009</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C69208</t>
-  </si>
-  <si>
-    <t>http://purl.allotrope.org/ontologies/role#AFRL_0000010</t>
-  </si>
-  <si>
-    <t>https://w3id.org/fair-genomes/resource/FG_0000002</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C68615</t>
-  </si>
-  <si>
-    <t>http://purl.org/dc/terms/valid</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C67073</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_001083</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_001330</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45262</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C48297</t>
-  </si>
-  <si>
     <t>dcat</t>
   </si>
   <si>
     <t>MESH</t>
   </si>
   <si>
+    <t>NCIT</t>
+  </si>
+  <si>
+    <t>EFO</t>
+  </si>
+  <si>
+    <t>EDAM</t>
+  </si>
+  <si>
+    <t>PATO</t>
+  </si>
+  <si>
+    <t>DUO</t>
+  </si>
+  <si>
+    <t>GENEPIO</t>
+  </si>
+  <si>
     <t>OBI</t>
   </si>
   <si>
-    <t>NCIT</t>
+    <t>GSSO</t>
+  </si>
+  <si>
+    <t>SNOMEDCT</t>
   </si>
   <si>
     <t>GO</t>
   </si>
   <si>
+    <t>FIX</t>
+  </si>
+  <si>
     <t>ExO</t>
   </si>
   <si>
-    <t>GENEPIO</t>
-  </si>
-  <si>
-    <t>SNOMEDCT</t>
-  </si>
-  <si>
-    <t>EFO</t>
-  </si>
-  <si>
-    <t>GSSO</t>
-  </si>
-  <si>
     <t>SCDO</t>
   </si>
   <si>
-    <t>EDAM</t>
-  </si>
-  <si>
-    <t>DUO</t>
-  </si>
-  <si>
-    <t>PATO</t>
-  </si>
-  <si>
-    <t>FIX</t>
+    <t>OMIABIS</t>
+  </si>
+  <si>
+    <t>reproduceme</t>
+  </si>
+  <si>
+    <t>DCMI</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>FG</t>
+  </si>
+  <si>
+    <t>AFO</t>
   </si>
   <si>
     <t>MS</t>
   </si>
   <si>
-    <t>OMIABIS</t>
-  </si>
-  <si>
-    <t>FG</t>
+    <t>SIO</t>
   </si>
   <si>
     <t>ICO</t>
   </si>
   <si>
+    <t>HL7</t>
+  </si>
+  <si>
     <t>Orphanet</t>
-  </si>
-  <si>
-    <t>RO</t>
-  </si>
-  <si>
-    <t>HL7</t>
-  </si>
-  <si>
-    <t>reproduceme</t>
-  </si>
-  <si>
-    <t>SIO</t>
-  </si>
-  <si>
-    <t>AFO</t>
-  </si>
-  <si>
-    <t>DCMI</t>
   </si>
   <si>
     <t>isAssociatedWith</t>
@@ -9282,7 +9282,7 @@
         <v>252</v>
       </c>
       <c r="C170" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D170" t="b">
         <v>0</v>
@@ -11389,10 +11389,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>595</v>
@@ -11409,10 +11409,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>596</v>
@@ -11429,16 +11429,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>597</v>
       </c>
       <c r="D7" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="E7" t="s">
         <v>765</v>
@@ -11449,16 +11449,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>598</v>
       </c>
       <c r="D8" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="E8" t="s">
         <v>765</v>
@@ -11469,16 +11469,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>599</v>
       </c>
       <c r="D9" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="E9" t="s">
         <v>765</v>
@@ -11489,16 +11489,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>600</v>
       </c>
       <c r="D10" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E10" t="s">
         <v>765</v>
@@ -11509,16 +11509,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>601</v>
       </c>
       <c r="D11" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="E11" t="s">
         <v>765</v>
@@ -11529,16 +11529,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>602</v>
       </c>
       <c r="D12" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E12" t="s">
         <v>765</v>
@@ -11549,16 +11549,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>603</v>
       </c>
       <c r="D13" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E13" t="s">
         <v>765</v>
@@ -11569,16 +11569,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>604</v>
       </c>
       <c r="D14" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="E14" t="s">
         <v>765</v>
@@ -11589,16 +11589,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>605</v>
       </c>
       <c r="D15" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="E15" t="s">
         <v>765</v>
@@ -11609,16 +11609,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>606</v>
       </c>
       <c r="D16" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E16" t="s">
         <v>765</v>
@@ -11629,16 +11629,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>607</v>
       </c>
       <c r="D17" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="E17" t="s">
         <v>765</v>
@@ -11649,16 +11649,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>608</v>
       </c>
       <c r="D18" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="E18" t="s">
         <v>765</v>
@@ -11669,16 +11669,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>609</v>
       </c>
       <c r="D19" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="E19" t="s">
         <v>765</v>
@@ -11689,16 +11689,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="B20" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>610</v>
       </c>
       <c r="D20" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="E20" t="s">
         <v>765</v>
@@ -11709,16 +11709,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>611</v>
       </c>
       <c r="D21" t="s">
-        <v>748</v>
+        <v>741</v>
       </c>
       <c r="E21" t="s">
         <v>765</v>
@@ -11729,16 +11729,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>612</v>
       </c>
       <c r="D22" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E22" t="s">
         <v>765</v>
@@ -11749,16 +11749,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>613</v>
       </c>
       <c r="D23" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E23" t="s">
         <v>765</v>
@@ -11769,16 +11769,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>614</v>
       </c>
       <c r="D24" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
       <c r="E24" t="s">
         <v>765</v>
@@ -11789,16 +11789,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>615</v>
       </c>
       <c r="D25" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="E25" t="s">
         <v>765</v>
@@ -11809,16 +11809,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>616</v>
       </c>
       <c r="D26" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="E26" t="s">
         <v>765</v>
@@ -11829,16 +11829,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>617</v>
       </c>
       <c r="D27" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E27" t="s">
         <v>765</v>
@@ -11849,16 +11849,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B28" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>618</v>
       </c>
       <c r="D28" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="E28" t="s">
         <v>765</v>
@@ -11869,16 +11869,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>619</v>
       </c>
       <c r="D29" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="E29" t="s">
         <v>765</v>
@@ -11889,16 +11889,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>620</v>
       </c>
       <c r="D30" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E30" t="s">
         <v>765</v>
@@ -11909,16 +11909,16 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>621</v>
       </c>
       <c r="D31" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E31" t="s">
         <v>765</v>
@@ -11929,16 +11929,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>622</v>
       </c>
       <c r="D32" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E32" t="s">
         <v>765</v>
@@ -11949,16 +11949,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B33" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>623</v>
       </c>
       <c r="D33" t="s">
-        <v>753</v>
+        <v>741</v>
       </c>
       <c r="E33" t="s">
         <v>765</v>
@@ -11969,16 +11969,16 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>624</v>
       </c>
       <c r="D34" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E34" t="s">
         <v>765</v>
@@ -11989,16 +11989,16 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>625</v>
       </c>
       <c r="D35" t="s">
-        <v>745</v>
+        <v>751</v>
       </c>
       <c r="E35" t="s">
         <v>765</v>
@@ -12009,16 +12009,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>626</v>
       </c>
       <c r="D36" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E36" t="s">
         <v>765</v>
@@ -12029,16 +12029,16 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="B37" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>627</v>
       </c>
       <c r="D37" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E37" t="s">
         <v>765</v>
@@ -12049,16 +12049,16 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>628</v>
       </c>
       <c r="D38" t="s">
-        <v>742</v>
+        <v>752</v>
       </c>
       <c r="E38" t="s">
         <v>765</v>
@@ -12069,16 +12069,16 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>629</v>
       </c>
       <c r="D39" t="s">
-        <v>742</v>
+        <v>747</v>
       </c>
       <c r="E39" t="s">
         <v>765</v>
@@ -12089,16 +12089,16 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>630</v>
       </c>
       <c r="D40" t="s">
-        <v>745</v>
+        <v>753</v>
       </c>
       <c r="E40" t="s">
         <v>765</v>
@@ -12109,16 +12109,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>430</v>
+        <v>121</v>
       </c>
       <c r="B41" t="s">
-        <v>430</v>
+        <v>121</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>631</v>
+        <v>594</v>
       </c>
       <c r="D41" t="s">
-        <v>754</v>
+        <v>740</v>
       </c>
       <c r="E41" t="s">
         <v>765</v>
@@ -12129,16 +12129,16 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>445</v>
+        <v>488</v>
       </c>
       <c r="B42" t="s">
-        <v>445</v>
+        <v>488</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D42" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
       <c r="E42" t="s">
         <v>765</v>
@@ -12149,16 +12149,16 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>522</v>
+        <v>491</v>
       </c>
       <c r="B43" t="s">
-        <v>522</v>
+        <v>491</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D43" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="E43" t="s">
         <v>765</v>
@@ -12169,16 +12169,16 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>487</v>
+        <v>440</v>
       </c>
       <c r="B44" t="s">
-        <v>487</v>
+        <v>440</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D44" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E44" t="s">
         <v>765</v>
@@ -12189,16 +12189,16 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>470</v>
       </c>
       <c r="B45" t="s">
-        <v>113</v>
+        <v>470</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>596</v>
+        <v>634</v>
       </c>
       <c r="D45" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E45" t="s">
         <v>765</v>
@@ -12209,16 +12209,16 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>435</v>
+        <v>504</v>
       </c>
       <c r="B46" t="s">
-        <v>435</v>
+        <v>504</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>635</v>
       </c>
       <c r="D46" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E46" t="s">
         <v>765</v>
@@ -12229,16 +12229,16 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>438</v>
+        <v>509</v>
       </c>
       <c r="B47" t="s">
-        <v>438</v>
+        <v>509</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>636</v>
       </c>
       <c r="D47" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="E47" t="s">
         <v>765</v>
@@ -12249,16 +12249,16 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>507</v>
+        <v>480</v>
       </c>
       <c r="B48" t="s">
-        <v>507</v>
+        <v>480</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>637</v>
       </c>
       <c r="D48" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E48" t="s">
         <v>765</v>
@@ -12269,16 +12269,16 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>513</v>
+        <v>483</v>
       </c>
       <c r="B49" t="s">
-        <v>513</v>
+        <v>483</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>638</v>
       </c>
       <c r="D49" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E49" t="s">
         <v>765</v>
@@ -12289,16 +12289,16 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>476</v>
+        <v>498</v>
       </c>
       <c r="B50" t="s">
-        <v>476</v>
+        <v>498</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>639</v>
       </c>
       <c r="D50" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E50" t="s">
         <v>765</v>
@@ -12309,16 +12309,16 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>512</v>
+        <v>132</v>
       </c>
       <c r="B51" t="s">
-        <v>512</v>
+        <v>132</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>640</v>
+        <v>607</v>
       </c>
       <c r="D51" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="E51" t="s">
         <v>765</v>
@@ -12329,13 +12329,13 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>492</v>
+        <v>525</v>
       </c>
       <c r="B52" t="s">
-        <v>492</v>
+        <v>525</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D52" t="s">
         <v>741</v>
@@ -12349,16 +12349,16 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>442</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>442</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>603</v>
+        <v>641</v>
       </c>
       <c r="D53" t="s">
-        <v>742</v>
+        <v>755</v>
       </c>
       <c r="E53" t="s">
         <v>765</v>
@@ -12369,16 +12369,16 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>479</v>
+        <v>456</v>
       </c>
       <c r="B54" t="s">
-        <v>479</v>
+        <v>456</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>642</v>
       </c>
       <c r="D54" t="s">
-        <v>742</v>
+        <v>756</v>
       </c>
       <c r="E54" t="s">
         <v>765</v>
@@ -12389,16 +12389,16 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="D55" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E55" t="s">
         <v>765</v>
@@ -12409,16 +12409,16 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>478</v>
       </c>
       <c r="B56" t="s">
-        <v>122</v>
+        <v>478</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>611</v>
+        <v>643</v>
       </c>
       <c r="D56" t="s">
-        <v>748</v>
+        <v>741</v>
       </c>
       <c r="E56" t="s">
         <v>765</v>
@@ -12429,16 +12429,16 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>428</v>
+        <v>469</v>
       </c>
       <c r="B57" t="s">
-        <v>428</v>
+        <v>469</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D57" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="E57" t="s">
         <v>765</v>
@@ -12449,16 +12449,16 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>107</v>
+        <v>449</v>
       </c>
       <c r="B58" t="s">
-        <v>107</v>
+        <v>449</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>617</v>
+        <v>645</v>
       </c>
       <c r="D58" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E58" t="s">
         <v>765</v>
@@ -12469,16 +12469,16 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>502</v>
+        <v>433</v>
       </c>
       <c r="B59" t="s">
-        <v>502</v>
+        <v>433</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="D59" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E59" t="s">
         <v>765</v>
@@ -12489,16 +12489,16 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>461</v>
+        <v>493</v>
       </c>
       <c r="B60" t="s">
-        <v>461</v>
+        <v>493</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="D60" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E60" t="s">
         <v>765</v>
@@ -12509,16 +12509,16 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>489</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>489</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>623</v>
+        <v>648</v>
       </c>
       <c r="D61" t="s">
-        <v>753</v>
+        <v>741</v>
       </c>
       <c r="E61" t="s">
         <v>765</v>
@@ -12529,16 +12529,16 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>434</v>
+        <v>476</v>
       </c>
       <c r="B62" t="s">
-        <v>434</v>
+        <v>476</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="D62" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E62" t="s">
         <v>765</v>
@@ -12549,16 +12549,16 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>506</v>
+        <v>516</v>
       </c>
       <c r="B63" t="s">
-        <v>506</v>
+        <v>516</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="D63" t="s">
-        <v>742</v>
+        <v>747</v>
       </c>
       <c r="E63" t="s">
         <v>765</v>
@@ -12569,16 +12569,16 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>471</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>471</v>
+        <v>126</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>648</v>
+        <v>619</v>
       </c>
       <c r="D64" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="E64" t="s">
         <v>765</v>
@@ -12589,16 +12589,16 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>498</v>
+        <v>108</v>
       </c>
       <c r="B65" t="s">
-        <v>498</v>
+        <v>108</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>649</v>
+        <v>617</v>
       </c>
       <c r="D65" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E65" t="s">
         <v>765</v>
@@ -12609,16 +12609,16 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>441</v>
+        <v>122</v>
       </c>
       <c r="B66" t="s">
-        <v>441</v>
+        <v>122</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="D66" t="s">
-        <v>742</v>
+        <v>748</v>
       </c>
       <c r="E66" t="s">
         <v>765</v>
@@ -12629,16 +12629,16 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>114</v>
+        <v>419</v>
       </c>
       <c r="B67" t="s">
-        <v>114</v>
+        <v>419</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>628</v>
+        <v>651</v>
       </c>
       <c r="D67" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E67" t="s">
         <v>765</v>
@@ -12649,16 +12649,16 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>108</v>
+        <v>463</v>
       </c>
       <c r="B68" t="s">
-        <v>108</v>
+        <v>463</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>629</v>
+        <v>652</v>
       </c>
       <c r="D68" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E68" t="s">
         <v>765</v>
@@ -12669,16 +12669,16 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>439</v>
+        <v>508</v>
       </c>
       <c r="B69" t="s">
-        <v>439</v>
+        <v>508</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="D69" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="E69" t="s">
         <v>765</v>
@@ -12689,16 +12689,16 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>126</v>
+        <v>436</v>
       </c>
       <c r="B70" t="s">
-        <v>126</v>
+        <v>436</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>630</v>
+        <v>654</v>
       </c>
       <c r="D70" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="E70" t="s">
         <v>765</v>
@@ -12709,16 +12709,16 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>425</v>
+        <v>446</v>
       </c>
       <c r="B71" t="s">
-        <v>425</v>
+        <v>446</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="D71" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E71" t="s">
         <v>765</v>
@@ -12729,16 +12729,16 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>421</v>
+        <v>119</v>
       </c>
       <c r="B72" t="s">
-        <v>421</v>
+        <v>119</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>653</v>
+        <v>622</v>
       </c>
       <c r="D72" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E72" t="s">
         <v>765</v>
@@ -12749,16 +12749,16 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>520</v>
+        <v>112</v>
       </c>
       <c r="B73" t="s">
-        <v>520</v>
+        <v>112</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>654</v>
+        <v>623</v>
       </c>
       <c r="D73" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E73" t="s">
         <v>765</v>
@@ -12769,16 +12769,16 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>446</v>
+        <v>133</v>
       </c>
       <c r="B74" t="s">
-        <v>446</v>
+        <v>133</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>655</v>
+        <v>627</v>
       </c>
       <c r="D74" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E74" t="s">
         <v>765</v>
@@ -12789,16 +12789,16 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B75" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>656</v>
       </c>
       <c r="D75" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E75" t="s">
         <v>765</v>
@@ -12809,16 +12809,16 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>508</v>
+        <v>454</v>
       </c>
       <c r="B76" t="s">
-        <v>508</v>
+        <v>454</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>657</v>
       </c>
       <c r="D76" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
       <c r="E76" t="s">
         <v>765</v>
@@ -12829,16 +12829,16 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>112</v>
+        <v>485</v>
       </c>
       <c r="B77" t="s">
-        <v>112</v>
+        <v>485</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>598</v>
+        <v>658</v>
       </c>
       <c r="D77" t="s">
-        <v>742</v>
+        <v>758</v>
       </c>
       <c r="E77" t="s">
         <v>765</v>
@@ -12849,16 +12849,16 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>484</v>
+        <v>507</v>
       </c>
       <c r="B78" t="s">
-        <v>484</v>
+        <v>507</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D78" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="E78" t="s">
         <v>765</v>
@@ -12869,16 +12869,16 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>463</v>
+        <v>517</v>
       </c>
       <c r="B79" t="s">
-        <v>463</v>
+        <v>517</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D79" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E79" t="s">
         <v>765</v>
@@ -12889,16 +12889,16 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>496</v>
+        <v>481</v>
       </c>
       <c r="B80" t="s">
-        <v>496</v>
+        <v>481</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="D80" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="E80" t="s">
         <v>765</v>
@@ -12909,16 +12909,16 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>128</v>
+        <v>522</v>
       </c>
       <c r="B81" t="s">
-        <v>128</v>
+        <v>522</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>602</v>
+        <v>662</v>
       </c>
       <c r="D81" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E81" t="s">
         <v>765</v>
@@ -12929,13 +12929,13 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="B82" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
       <c r="D82" t="s">
         <v>742</v>
@@ -12949,16 +12949,16 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="B83" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="D83" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="E83" t="s">
         <v>765</v>
@@ -12969,16 +12969,16 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>477</v>
+        <v>506</v>
       </c>
       <c r="B84" t="s">
-        <v>477</v>
+        <v>506</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="D84" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E84" t="s">
         <v>765</v>
@@ -12989,16 +12989,16 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>466</v>
+        <v>430</v>
       </c>
       <c r="B85" t="s">
-        <v>466</v>
+        <v>430</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="D85" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="E85" t="s">
         <v>765</v>
@@ -13009,16 +13009,16 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>129</v>
+        <v>437</v>
       </c>
       <c r="B86" t="s">
-        <v>129</v>
+        <v>437</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>607</v>
+        <v>666</v>
       </c>
       <c r="D86" t="s">
-        <v>742</v>
+        <v>761</v>
       </c>
       <c r="E86" t="s">
         <v>765</v>
@@ -13029,16 +13029,16 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>486</v>
+        <v>120</v>
       </c>
       <c r="B87" t="s">
-        <v>486</v>
+        <v>120</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>664</v>
+        <v>598</v>
       </c>
       <c r="D87" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="E87" t="s">
         <v>765</v>
@@ -13049,16 +13049,16 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>106</v>
+        <v>500</v>
       </c>
       <c r="B88" t="s">
-        <v>106</v>
+        <v>500</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>612</v>
+        <v>667</v>
       </c>
       <c r="D88" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E88" t="s">
         <v>765</v>
@@ -13069,16 +13069,16 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>462</v>
+        <v>510</v>
       </c>
       <c r="B89" t="s">
-        <v>462</v>
+        <v>510</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="D89" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E89" t="s">
         <v>765</v>
@@ -13089,16 +13089,16 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
       <c r="B90" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="D90" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
       <c r="E90" t="s">
         <v>765</v>
@@ -13109,16 +13109,16 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="B91" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="D91" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E91" t="s">
         <v>765</v>
@@ -13129,16 +13129,16 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>489</v>
+        <v>461</v>
       </c>
       <c r="B92" t="s">
-        <v>489</v>
+        <v>461</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="D92" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E92" t="s">
         <v>765</v>
@@ -13149,16 +13149,16 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>504</v>
+        <v>518</v>
       </c>
       <c r="B93" t="s">
-        <v>504</v>
+        <v>518</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="D93" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E93" t="s">
         <v>765</v>
@@ -13169,16 +13169,16 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>473</v>
+        <v>109</v>
       </c>
       <c r="B94" t="s">
-        <v>473</v>
+        <v>109</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>670</v>
+        <v>612</v>
       </c>
       <c r="D94" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E94" t="s">
         <v>765</v>
@@ -13189,16 +13189,16 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>485</v>
+        <v>453</v>
       </c>
       <c r="B95" t="s">
-        <v>485</v>
+        <v>453</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="D95" t="s">
-        <v>756</v>
+        <v>762</v>
       </c>
       <c r="E95" t="s">
         <v>765</v>
@@ -13209,16 +13209,16 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>433</v>
+        <v>524</v>
       </c>
       <c r="B96" t="s">
-        <v>433</v>
+        <v>524</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="D96" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E96" t="s">
         <v>765</v>
@@ -13229,16 +13229,16 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>509</v>
+        <v>451</v>
       </c>
       <c r="B97" t="s">
-        <v>509</v>
+        <v>451</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="D97" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
       <c r="E97" t="s">
         <v>765</v>
@@ -13249,16 +13249,16 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>426</v>
+        <v>479</v>
       </c>
       <c r="B98" t="s">
-        <v>426</v>
+        <v>479</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="D98" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E98" t="s">
         <v>765</v>
@@ -13269,16 +13269,16 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>501</v>
+        <v>131</v>
       </c>
       <c r="B99" t="s">
-        <v>501</v>
+        <v>131</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>675</v>
+        <v>625</v>
       </c>
       <c r="D99" t="s">
-        <v>742</v>
+        <v>751</v>
       </c>
       <c r="E99" t="s">
         <v>765</v>
@@ -13289,16 +13289,16 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>420</v>
+        <v>455</v>
       </c>
       <c r="B100" t="s">
-        <v>420</v>
+        <v>455</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="D100" t="s">
-        <v>742</v>
+        <v>762</v>
       </c>
       <c r="E100" t="s">
         <v>765</v>
@@ -13309,16 +13309,16 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>482</v>
+        <v>464</v>
       </c>
       <c r="B101" t="s">
-        <v>482</v>
+        <v>464</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D101" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E101" t="s">
         <v>765</v>
@@ -13329,16 +13329,16 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>118</v>
+        <v>418</v>
       </c>
       <c r="B102" t="s">
-        <v>118</v>
+        <v>418</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>627</v>
+        <v>679</v>
       </c>
       <c r="D102" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E102" t="s">
         <v>765</v>
@@ -13349,13 +13349,13 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>516</v>
+        <v>499</v>
       </c>
       <c r="B103" t="s">
-        <v>516</v>
+        <v>499</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="D103" t="s">
         <v>741</v>
@@ -13369,16 +13369,16 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>497</v>
+        <v>465</v>
       </c>
       <c r="B104" t="s">
-        <v>497</v>
+        <v>465</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="D104" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E104" t="s">
         <v>765</v>
@@ -13389,13 +13389,13 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>130</v>
+        <v>458</v>
       </c>
       <c r="B105" t="s">
-        <v>130</v>
+        <v>458</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>604</v>
+        <v>682</v>
       </c>
       <c r="D105" t="s">
         <v>745</v>
@@ -13409,16 +13409,16 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="B106" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="D106" t="s">
-        <v>759</v>
+        <v>741</v>
       </c>
       <c r="E106" t="s">
         <v>765</v>
@@ -13429,16 +13429,16 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>121</v>
+        <v>477</v>
       </c>
       <c r="B107" t="s">
-        <v>121</v>
+        <v>477</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>594</v>
+        <v>684</v>
       </c>
       <c r="D107" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E107" t="s">
         <v>765</v>
@@ -13449,13 +13449,13 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>124</v>
+        <v>487</v>
       </c>
       <c r="B108" t="s">
-        <v>124</v>
+        <v>487</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>595</v>
+        <v>685</v>
       </c>
       <c r="D108" t="s">
         <v>741</v>
@@ -13469,16 +13469,16 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>525</v>
+        <v>448</v>
       </c>
       <c r="B109" t="s">
-        <v>525</v>
+        <v>448</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>681</v>
+        <v>686</v>
       </c>
       <c r="D109" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E109" t="s">
         <v>765</v>
@@ -13489,16 +13489,16 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>467</v>
+        <v>123</v>
       </c>
       <c r="B110" t="s">
-        <v>467</v>
+        <v>123</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>682</v>
+        <v>599</v>
       </c>
       <c r="D110" t="s">
-        <v>760</v>
+        <v>744</v>
       </c>
       <c r="E110" t="s">
         <v>765</v>
@@ -13509,16 +13509,16 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="B111" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="D111" t="s">
-        <v>742</v>
+        <v>761</v>
       </c>
       <c r="E111" t="s">
         <v>765</v>
@@ -13529,16 +13529,16 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>429</v>
+        <v>118</v>
       </c>
       <c r="B112" t="s">
-        <v>429</v>
+        <v>118</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>684</v>
+        <v>601</v>
       </c>
       <c r="D112" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E112" t="s">
         <v>765</v>
@@ -13549,16 +13549,16 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>127</v>
+        <v>460</v>
       </c>
       <c r="B113" t="s">
-        <v>127</v>
+        <v>460</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>597</v>
+        <v>688</v>
       </c>
       <c r="D113" t="s">
-        <v>743</v>
+        <v>762</v>
       </c>
       <c r="E113" t="s">
         <v>765</v>
@@ -13569,16 +13569,16 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>469</v>
+        <v>426</v>
       </c>
       <c r="B114" t="s">
-        <v>469</v>
+        <v>426</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c r="D114" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E114" t="s">
         <v>765</v>
@@ -13589,16 +13589,16 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>478</v>
+        <v>494</v>
       </c>
       <c r="B115" t="s">
-        <v>478</v>
+        <v>494</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="D115" t="s">
-        <v>742</v>
+        <v>758</v>
       </c>
       <c r="E115" t="s">
         <v>765</v>
@@ -13609,16 +13609,16 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>518</v>
+        <v>502</v>
       </c>
       <c r="B116" t="s">
-        <v>518</v>
+        <v>502</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="D116" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E116" t="s">
         <v>765</v>
@@ -13629,16 +13629,16 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>472</v>
+        <v>496</v>
       </c>
       <c r="B117" t="s">
-        <v>472</v>
+        <v>496</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="D117" t="s">
-        <v>742</v>
+        <v>758</v>
       </c>
       <c r="E117" t="s">
         <v>765</v>
@@ -13649,13 +13649,13 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="B118" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="D118" t="s">
         <v>742</v>
@@ -13669,16 +13669,16 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>451</v>
+        <v>521</v>
       </c>
       <c r="B119" t="s">
-        <v>451</v>
+        <v>521</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="D119" t="s">
-        <v>742</v>
+        <v>761</v>
       </c>
       <c r="E119" t="s">
         <v>765</v>
@@ -13689,16 +13689,16 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>483</v>
+        <v>513</v>
       </c>
       <c r="B120" t="s">
-        <v>483</v>
+        <v>513</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
       <c r="D120" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E120" t="s">
         <v>765</v>
@@ -13709,16 +13709,16 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>427</v>
+        <v>503</v>
       </c>
       <c r="B121" t="s">
-        <v>427</v>
+        <v>503</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="D121" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E121" t="s">
         <v>765</v>
@@ -13729,16 +13729,16 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>470</v>
+        <v>511</v>
       </c>
       <c r="B122" t="s">
-        <v>470</v>
+        <v>511</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="D122" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E122" t="s">
         <v>765</v>
@@ -13749,16 +13749,16 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>517</v>
+        <v>501</v>
       </c>
       <c r="B123" t="s">
-        <v>517</v>
+        <v>501</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="D123" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E123" t="s">
         <v>765</v>
@@ -13769,16 +13769,16 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>110</v>
+        <v>424</v>
       </c>
       <c r="B124" t="s">
-        <v>110</v>
+        <v>424</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>610</v>
+        <v>699</v>
       </c>
       <c r="D124" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="E124" t="s">
         <v>765</v>
@@ -13789,16 +13789,16 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B125" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>695</v>
+        <v>700</v>
       </c>
       <c r="D125" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E125" t="s">
         <v>765</v>
@@ -13809,16 +13809,16 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>480</v>
+        <v>107</v>
       </c>
       <c r="B126" t="s">
-        <v>480</v>
+        <v>107</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>696</v>
+        <v>613</v>
       </c>
       <c r="D126" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E126" t="s">
         <v>765</v>
@@ -13829,16 +13829,16 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="B127" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="D127" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E127" t="s">
         <v>765</v>
@@ -13849,16 +13849,16 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>515</v>
+        <v>472</v>
       </c>
       <c r="B128" t="s">
-        <v>515</v>
+        <v>472</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>698</v>
+        <v>702</v>
       </c>
       <c r="D128" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E128" t="s">
         <v>765</v>
@@ -13869,16 +13869,16 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="B129" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="D129" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="E129" t="s">
         <v>765</v>
@@ -13889,16 +13889,16 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>440</v>
+        <v>512</v>
       </c>
       <c r="B130" t="s">
-        <v>440</v>
+        <v>512</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
       <c r="D130" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E130" t="s">
         <v>765</v>
@@ -13909,16 +13909,16 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>448</v>
+        <v>515</v>
       </c>
       <c r="B131" t="s">
-        <v>448</v>
+        <v>515</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>701</v>
+        <v>705</v>
       </c>
       <c r="D131" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E131" t="s">
         <v>765</v>
@@ -13929,16 +13929,16 @@
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="B132" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="D132" t="s">
-        <v>761</v>
+        <v>741</v>
       </c>
       <c r="E132" t="s">
         <v>765</v>
@@ -13949,16 +13949,16 @@
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>123</v>
+        <v>475</v>
       </c>
       <c r="B133" t="s">
-        <v>123</v>
+        <v>475</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>621</v>
+        <v>707</v>
       </c>
       <c r="D133" t="s">
-        <v>752</v>
+        <v>742</v>
       </c>
       <c r="E133" t="s">
         <v>765</v>
@@ -13969,16 +13969,16 @@
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>431</v>
+        <v>447</v>
       </c>
       <c r="B134" t="s">
-        <v>431</v>
+        <v>447</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
       <c r="D134" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E134" t="s">
         <v>765</v>
@@ -13989,16 +13989,16 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="s">
-        <v>125</v>
+        <v>473</v>
       </c>
       <c r="B135" t="s">
-        <v>125</v>
+        <v>473</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>622</v>
+        <v>709</v>
       </c>
       <c r="D135" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E135" t="s">
         <v>765</v>
@@ -14009,16 +14009,16 @@
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B136" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>624</v>
       </c>
       <c r="D136" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E136" t="s">
         <v>765</v>
@@ -14029,16 +14029,16 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" t="s">
-        <v>495</v>
+        <v>467</v>
       </c>
       <c r="B137" t="s">
-        <v>495</v>
+        <v>467</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>704</v>
+        <v>710</v>
       </c>
       <c r="D137" t="s">
-        <v>745</v>
+        <v>763</v>
       </c>
       <c r="E137" t="s">
         <v>765</v>
@@ -14049,16 +14049,16 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>453</v>
+        <v>106</v>
       </c>
       <c r="B138" t="s">
-        <v>453</v>
+        <v>106</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>705</v>
+        <v>626</v>
       </c>
       <c r="D138" t="s">
-        <v>757</v>
+        <v>741</v>
       </c>
       <c r="E138" t="s">
         <v>765</v>
@@ -14069,16 +14069,16 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>475</v>
+        <v>428</v>
       </c>
       <c r="B139" t="s">
-        <v>475</v>
+        <v>428</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>706</v>
+        <v>711</v>
       </c>
       <c r="D139" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E139" t="s">
         <v>765</v>
@@ -14089,16 +14089,16 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>132</v>
+        <v>482</v>
       </c>
       <c r="B140" t="s">
-        <v>132</v>
+        <v>482</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>625</v>
+        <v>712</v>
       </c>
       <c r="D140" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="E140" t="s">
         <v>765</v>
@@ -14109,16 +14109,16 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>452</v>
+        <v>486</v>
       </c>
       <c r="B141" t="s">
-        <v>452</v>
+        <v>486</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
       <c r="D141" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E141" t="s">
         <v>765</v>
@@ -14129,16 +14129,16 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>455</v>
+        <v>423</v>
       </c>
       <c r="B142" t="s">
-        <v>455</v>
+        <v>423</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c r="D142" t="s">
-        <v>757</v>
+        <v>741</v>
       </c>
       <c r="E142" t="s">
         <v>765</v>
@@ -14149,16 +14149,16 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>493</v>
+        <v>421</v>
       </c>
       <c r="B143" t="s">
-        <v>493</v>
+        <v>421</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="D143" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E143" t="s">
         <v>765</v>
@@ -14169,16 +14169,16 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>511</v>
+        <v>441</v>
       </c>
       <c r="B144" t="s">
-        <v>511</v>
+        <v>441</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="D144" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E144" t="s">
         <v>765</v>
@@ -14189,16 +14189,16 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>491</v>
+        <v>431</v>
       </c>
       <c r="B145" t="s">
-        <v>491</v>
+        <v>431</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="D145" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="E145" t="s">
         <v>765</v>
@@ -14209,16 +14209,16 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>422</v>
+        <v>457</v>
       </c>
       <c r="B146" t="s">
-        <v>422</v>
+        <v>457</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="D146" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E146" t="s">
         <v>765</v>
@@ -14229,16 +14229,16 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>505</v>
+        <v>134</v>
       </c>
       <c r="B147" t="s">
-        <v>505</v>
+        <v>134</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>713</v>
+        <v>597</v>
       </c>
       <c r="D147" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E147" t="s">
         <v>765</v>
@@ -14249,16 +14249,16 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>510</v>
+        <v>452</v>
       </c>
       <c r="B148" t="s">
-        <v>510</v>
+        <v>452</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>714</v>
+        <v>719</v>
       </c>
       <c r="D148" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E148" t="s">
         <v>765</v>
@@ -14269,16 +14269,16 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
-        <v>447</v>
+        <v>462</v>
       </c>
       <c r="B149" t="s">
-        <v>447</v>
+        <v>462</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>715</v>
+        <v>720</v>
       </c>
       <c r="D149" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E149" t="s">
         <v>765</v>
@@ -14289,16 +14289,16 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
-        <v>468</v>
+        <v>113</v>
       </c>
       <c r="B150" t="s">
-        <v>468</v>
+        <v>113</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>716</v>
+        <v>602</v>
       </c>
       <c r="D150" t="s">
-        <v>760</v>
+        <v>741</v>
       </c>
       <c r="E150" t="s">
         <v>765</v>
@@ -14309,16 +14309,16 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B151" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
       <c r="D151" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E151" t="s">
         <v>765</v>
@@ -14329,16 +14329,16 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
-        <v>459</v>
+        <v>116</v>
       </c>
       <c r="B152" t="s">
-        <v>459</v>
+        <v>116</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>718</v>
+        <v>605</v>
       </c>
       <c r="D152" t="s">
-        <v>762</v>
+        <v>745</v>
       </c>
       <c r="E152" t="s">
         <v>765</v>
@@ -14349,16 +14349,16 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>457</v>
+        <v>471</v>
       </c>
       <c r="B153" t="s">
-        <v>457</v>
+        <v>471</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="D153" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="E153" t="s">
         <v>765</v>
@@ -14369,16 +14369,16 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
-        <v>443</v>
+        <v>490</v>
       </c>
       <c r="B154" t="s">
-        <v>443</v>
+        <v>490</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="D154" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
       <c r="E154" t="s">
         <v>765</v>
@@ -14389,16 +14389,16 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="B155" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="D155" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="E155" t="s">
         <v>765</v>
@@ -14409,16 +14409,16 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>444</v>
+        <v>129</v>
       </c>
       <c r="B156" t="s">
-        <v>444</v>
+        <v>129</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>722</v>
+        <v>610</v>
       </c>
       <c r="D156" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E156" t="s">
         <v>765</v>
@@ -14429,16 +14429,16 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="B157" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="D157" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E157" t="s">
         <v>765</v>
@@ -14449,16 +14449,16 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B158" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>600</v>
+        <v>611</v>
       </c>
       <c r="D158" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E158" t="s">
         <v>765</v>
@@ -14469,16 +14469,16 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>464</v>
+        <v>474</v>
       </c>
       <c r="B159" t="s">
-        <v>464</v>
+        <v>474</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="D159" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E159" t="s">
         <v>765</v>
@@ -14489,16 +14489,16 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
-        <v>474</v>
+        <v>443</v>
       </c>
       <c r="B160" t="s">
-        <v>474</v>
+        <v>443</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="D160" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="E160" t="s">
         <v>765</v>
@@ -14509,16 +14509,16 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>418</v>
+        <v>450</v>
       </c>
       <c r="B161" t="s">
-        <v>418</v>
+        <v>450</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="D161" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E161" t="s">
         <v>765</v>
@@ -14529,16 +14529,16 @@
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
-        <v>514</v>
+        <v>432</v>
       </c>
       <c r="B162" t="s">
-        <v>514</v>
+        <v>432</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="D162" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E162" t="s">
         <v>765</v>
@@ -14549,13 +14549,13 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
-        <v>465</v>
+        <v>130</v>
       </c>
       <c r="B163" t="s">
-        <v>465</v>
+        <v>130</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>728</v>
+        <v>614</v>
       </c>
       <c r="D163" t="s">
         <v>746</v>
@@ -14569,16 +14569,16 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
-        <v>450</v>
+        <v>115</v>
       </c>
       <c r="B164" t="s">
-        <v>450</v>
+        <v>115</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>729</v>
+        <v>615</v>
       </c>
       <c r="D164" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E164" t="s">
         <v>765</v>
@@ -14589,16 +14589,16 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>481</v>
+        <v>492</v>
       </c>
       <c r="B165" t="s">
-        <v>481</v>
+        <v>492</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>730</v>
       </c>
       <c r="D165" t="s">
-        <v>763</v>
+        <v>747</v>
       </c>
       <c r="E165" t="s">
         <v>765</v>
@@ -14609,16 +14609,16 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
-        <v>494</v>
+        <v>523</v>
       </c>
       <c r="B166" t="s">
-        <v>494</v>
+        <v>523</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>731</v>
       </c>
       <c r="D166" t="s">
-        <v>756</v>
+        <v>741</v>
       </c>
       <c r="E166" t="s">
         <v>765</v>
@@ -14629,16 +14629,16 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="B167" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>732</v>
       </c>
       <c r="D167" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E167" t="s">
         <v>765</v>
@@ -14649,13 +14649,13 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B168" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="D168" t="s">
         <v>750</v>
@@ -14669,16 +14669,16 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
-        <v>456</v>
+        <v>505</v>
       </c>
       <c r="B169" t="s">
-        <v>456</v>
+        <v>505</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>733</v>
       </c>
       <c r="D169" t="s">
-        <v>764</v>
+        <v>741</v>
       </c>
       <c r="E169" t="s">
         <v>765</v>
@@ -14689,16 +14689,16 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" t="s">
-        <v>116</v>
+        <v>444</v>
       </c>
       <c r="B170" t="s">
-        <v>116</v>
+        <v>444</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>620</v>
+        <v>734</v>
       </c>
       <c r="D170" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
       <c r="E170" t="s">
         <v>765</v>
@@ -14709,16 +14709,16 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" t="s">
-        <v>488</v>
+        <v>468</v>
       </c>
       <c r="B171" t="s">
-        <v>488</v>
+        <v>468</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="D171" t="s">
-        <v>742</v>
+        <v>763</v>
       </c>
       <c r="E171" t="s">
         <v>765</v>
@@ -14729,16 +14729,16 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" t="s">
-        <v>521</v>
+        <v>438</v>
       </c>
       <c r="B172" t="s">
-        <v>521</v>
+        <v>438</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="D172" t="s">
-        <v>762</v>
+        <v>741</v>
       </c>
       <c r="E172" t="s">
         <v>765</v>
@@ -14749,16 +14749,16 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="B173" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="D173" t="s">
-        <v>762</v>
+        <v>741</v>
       </c>
       <c r="E173" t="s">
         <v>765</v>
@@ -14769,16 +14769,16 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="B174" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="D174" t="s">
-        <v>742</v>
+        <v>764</v>
       </c>
       <c r="E174" t="s">
         <v>765</v>
@@ -14789,16 +14789,16 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" t="s">
-        <v>499</v>
+        <v>124</v>
       </c>
       <c r="B175" t="s">
-        <v>499</v>
+        <v>124</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>738</v>
+        <v>629</v>
       </c>
       <c r="D175" t="s">
-        <v>742</v>
+        <v>747</v>
       </c>
       <c r="E175" t="s">
         <v>765</v>
@@ -14911,7 +14911,7 @@
     <hyperlink ref="F51" r:id="rId100" location="isAssociatedWith"/>
     <hyperlink ref="C52" r:id="rId101"/>
     <hyperlink ref="F52" r:id="rId102" location="isAssociatedWith"/>
-    <hyperlink ref="C53" r:id="rId103"/>
+    <hyperlink ref="C53" r:id="rId103" location="wasUpdatedBy"/>
     <hyperlink ref="F53" r:id="rId104" location="isAssociatedWith"/>
     <hyperlink ref="C54" r:id="rId105"/>
     <hyperlink ref="F54" r:id="rId106" location="isAssociatedWith"/>
@@ -14965,7 +14965,7 @@
     <hyperlink ref="F78" r:id="rId154" location="isAssociatedWith"/>
     <hyperlink ref="C79" r:id="rId155"/>
     <hyperlink ref="F79" r:id="rId156" location="isAssociatedWith"/>
-    <hyperlink ref="C80" r:id="rId157"/>
+    <hyperlink ref="C80" r:id="rId157" location="AFRL_0000010"/>
     <hyperlink ref="F80" r:id="rId158" location="isAssociatedWith"/>
     <hyperlink ref="C81" r:id="rId159"/>
     <hyperlink ref="F81" r:id="rId160" location="isAssociatedWith"/>
@@ -15069,7 +15069,7 @@
     <hyperlink ref="F130" r:id="rId258" location="isAssociatedWith"/>
     <hyperlink ref="C131" r:id="rId259"/>
     <hyperlink ref="F131" r:id="rId260" location="isAssociatedWith"/>
-    <hyperlink ref="C132" r:id="rId261" location="wasUpdatedBy"/>
+    <hyperlink ref="C132" r:id="rId261"/>
     <hyperlink ref="F132" r:id="rId262" location="isAssociatedWith"/>
     <hyperlink ref="C133" r:id="rId263"/>
     <hyperlink ref="F133" r:id="rId264" location="isAssociatedWith"/>
@@ -15135,7 +15135,7 @@
     <hyperlink ref="F163" r:id="rId324" location="isAssociatedWith"/>
     <hyperlink ref="C164" r:id="rId325"/>
     <hyperlink ref="F164" r:id="rId326" location="isAssociatedWith"/>
-    <hyperlink ref="C165" r:id="rId327" location="AFRL_0000010"/>
+    <hyperlink ref="C165" r:id="rId327"/>
     <hyperlink ref="F165" r:id="rId328" location="isAssociatedWith"/>
     <hyperlink ref="C166" r:id="rId329"/>
     <hyperlink ref="F166" r:id="rId330" location="isAssociatedWith"/>

</xml_diff>